<commit_message>
Actualización de fechas del equipo de desarrollo en el Registro de estado de progreso
Actualización de las fechas de las actividades del equipo de desarrollo hasta hoy 30-08-2019
</commit_message>
<xml_diff>
--- a/Documentos para el proyecto de Sanambiente/Registro de estado de progreso.xlsx
+++ b/Documentos para el proyecto de Sanambiente/Registro de estado de progreso.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aarón Gomez\Documents\GitHub\Proyecto-Sanambiente\Documentos para el proyecto de Sanambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE93CF51-281B-4E7E-A8D0-413E81A1F86B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8AA9C8-7204-4484-B38D-C3CD3485DF8A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2839,32 +2839,11 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2884,11 +2863,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2897,6 +2897,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2924,15 +2933,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6813,8 +6813,8 @@
   </sheetPr>
   <dimension ref="A1:AD1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F107" sqref="F107"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F117" sqref="F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -6857,23 +6857,23 @@
       <c r="C2" s="124" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="91" t="s">
+      <c r="D2" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="91" t="s">
+      <c r="E2" s="76" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="120" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="121"/>
-      <c r="H2" s="91" t="s">
+      <c r="H2" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="91" t="s">
+      <c r="I2" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="91" t="s">
+      <c r="J2" s="76" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="65"/>
@@ -6897,17 +6897,17 @@
       <c r="A3" s="123"/>
       <c r="B3" s="123"/>
       <c r="C3" s="125"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
       <c r="F3" s="56" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
       <c r="K3" s="65"/>
       <c r="M3" s="114"/>
       <c r="N3" s="115"/>
@@ -6929,13 +6929,13 @@
       <c r="A4" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="88">
+      <c r="B4" s="81">
         <v>1</v>
       </c>
-      <c r="C4" s="76">
+      <c r="C4" s="90">
         <v>43466</v>
       </c>
-      <c r="D4" s="82">
+      <c r="D4" s="84">
         <v>43638</v>
       </c>
       <c r="E4" s="54">
@@ -6943,13 +6943,13 @@
       </c>
       <c r="F4" s="27"/>
       <c r="G4" s="43"/>
-      <c r="H4" s="82">
+      <c r="H4" s="84">
         <v>43639</v>
       </c>
-      <c r="I4" s="88">
+      <c r="I4" s="81">
         <v>6</v>
       </c>
-      <c r="J4" s="88">
+      <c r="J4" s="81">
         <v>7</v>
       </c>
       <c r="K4" s="65"/>
@@ -6963,17 +6963,17 @@
     </row>
     <row r="5" spans="1:30" ht="13.2" customHeight="1">
       <c r="A5" s="109"/>
-      <c r="B5" s="89"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="83"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="85"/>
       <c r="E5" s="54">
         <v>43639</v>
       </c>
       <c r="F5" s="53"/>
       <c r="G5" s="26"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="82"/>
       <c r="K5" s="65"/>
       <c r="M5" s="114"/>
       <c r="N5" s="115"/>
@@ -6985,15 +6985,15 @@
     </row>
     <row r="6" spans="1:30" ht="13.2" customHeight="1">
       <c r="A6" s="109"/>
-      <c r="B6" s="89"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="83"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="85"/>
       <c r="E6" s="54"/>
       <c r="F6" s="53"/>
       <c r="G6" s="53"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="89"/>
-      <c r="J6" s="89"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="82"/>
       <c r="K6" s="65"/>
       <c r="M6" s="117"/>
       <c r="N6" s="118"/>
@@ -7005,15 +7005,15 @@
     </row>
     <row r="7" spans="1:30" ht="13.2" customHeight="1">
       <c r="A7" s="109"/>
-      <c r="B7" s="89"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="83"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="85"/>
       <c r="E7" s="54"/>
       <c r="F7" s="53"/>
       <c r="G7" s="53"/>
-      <c r="H7" s="83"/>
-      <c r="I7" s="89"/>
-      <c r="J7" s="89"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
       <c r="K7" s="65"/>
       <c r="Q7" s="10"/>
       <c r="R7" s="10"/>
@@ -7024,17 +7024,17 @@
     </row>
     <row r="8" spans="1:30" ht="13.2" customHeight="1">
       <c r="A8" s="109"/>
-      <c r="B8" s="89"/>
-      <c r="C8" s="76">
+      <c r="B8" s="82"/>
+      <c r="C8" s="90">
         <v>43497</v>
       </c>
-      <c r="D8" s="83"/>
+      <c r="D8" s="85"/>
       <c r="E8" s="54"/>
       <c r="F8" s="53"/>
       <c r="G8" s="53"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="89"/>
-      <c r="J8" s="89"/>
+      <c r="H8" s="85"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="82"/>
       <c r="K8" s="65"/>
       <c r="Q8" s="10"/>
       <c r="R8" s="10"/>
@@ -7045,15 +7045,15 @@
     </row>
     <row r="9" spans="1:30" ht="13.2" customHeight="1">
       <c r="A9" s="109"/>
-      <c r="B9" s="89"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="83"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="91"/>
+      <c r="D9" s="85"/>
       <c r="E9" s="54"/>
       <c r="F9" s="53"/>
       <c r="G9" s="53"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="89"/>
-      <c r="J9" s="89"/>
+      <c r="H9" s="85"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="82"/>
       <c r="K9" s="65"/>
       <c r="Q9" s="10"/>
       <c r="R9" s="10"/>
@@ -7064,15 +7064,15 @@
     </row>
     <row r="10" spans="1:30" ht="13.2" customHeight="1">
       <c r="A10" s="109"/>
-      <c r="B10" s="89"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="83"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="85"/>
       <c r="E10" s="54"/>
       <c r="F10" s="53"/>
       <c r="G10" s="53"/>
-      <c r="H10" s="83"/>
-      <c r="I10" s="89"/>
-      <c r="J10" s="89"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="82"/>
       <c r="K10" s="65"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
@@ -7083,15 +7083,15 @@
     </row>
     <row r="11" spans="1:30" ht="13.2" customHeight="1">
       <c r="A11" s="109"/>
-      <c r="B11" s="90"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="84"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="86"/>
       <c r="E11" s="54"/>
       <c r="F11" s="53"/>
       <c r="G11" s="53"/>
-      <c r="H11" s="84"/>
-      <c r="I11" s="90"/>
-      <c r="J11" s="90"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="83"/>
+      <c r="J11" s="83"/>
       <c r="K11" s="65"/>
       <c r="Q11" s="10"/>
       <c r="R11" s="10"/>
@@ -7102,15 +7102,15 @@
     </row>
     <row r="12" spans="1:30" ht="13.2" customHeight="1">
       <c r="A12" s="109"/>
-      <c r="B12" s="85"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="86"/>
-      <c r="I12" s="86"/>
-      <c r="J12" s="87"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="79"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="80"/>
       <c r="K12" s="65"/>
       <c r="Q12" s="10"/>
       <c r="R12" s="10"/>
@@ -7121,13 +7121,13 @@
     </row>
     <row r="13" spans="1:30" ht="13.2" customHeight="1">
       <c r="A13" s="109"/>
-      <c r="B13" s="88">
+      <c r="B13" s="81">
         <v>2</v>
       </c>
-      <c r="C13" s="76">
+      <c r="C13" s="90">
         <v>43467</v>
       </c>
-      <c r="D13" s="82">
+      <c r="D13" s="84">
         <v>43641</v>
       </c>
       <c r="E13" s="54">
@@ -7135,13 +7135,13 @@
       </c>
       <c r="F13" s="44"/>
       <c r="G13" s="40"/>
-      <c r="H13" s="82">
+      <c r="H13" s="84">
         <v>43640</v>
       </c>
-      <c r="I13" s="88">
+      <c r="I13" s="81">
         <v>3</v>
       </c>
-      <c r="J13" s="88">
+      <c r="J13" s="81">
         <v>2</v>
       </c>
       <c r="K13" s="65"/>
@@ -7155,15 +7155,15 @@
     </row>
     <row r="14" spans="1:30" ht="13.2" customHeight="1">
       <c r="A14" s="109"/>
-      <c r="B14" s="89"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="83"/>
+      <c r="B14" s="82"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="85"/>
       <c r="E14" s="54"/>
       <c r="F14" s="51"/>
       <c r="G14" s="53"/>
-      <c r="H14" s="83"/>
-      <c r="I14" s="89"/>
-      <c r="J14" s="89"/>
+      <c r="H14" s="85"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="82"/>
       <c r="K14" s="65"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
@@ -7179,15 +7179,15 @@
     </row>
     <row r="15" spans="1:30" ht="13.2" customHeight="1">
       <c r="A15" s="109"/>
-      <c r="B15" s="89"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="83"/>
+      <c r="B15" s="82"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="85"/>
       <c r="E15" s="54"/>
       <c r="F15" s="53"/>
       <c r="G15" s="53"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="89"/>
-      <c r="J15" s="89"/>
+      <c r="H15" s="85"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="82"/>
       <c r="K15" s="65"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
@@ -7203,15 +7203,15 @@
     </row>
     <row r="16" spans="1:30" ht="13.2" customHeight="1">
       <c r="A16" s="109"/>
-      <c r="B16" s="89"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="84"/>
+      <c r="B16" s="82"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="86"/>
       <c r="E16" s="53"/>
       <c r="F16" s="53"/>
       <c r="G16" s="53"/>
-      <c r="H16" s="84"/>
-      <c r="I16" s="89"/>
-      <c r="J16" s="90"/>
+      <c r="H16" s="86"/>
+      <c r="I16" s="82"/>
+      <c r="J16" s="83"/>
       <c r="K16" s="65"/>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
@@ -7227,11 +7227,11 @@
     </row>
     <row r="17" spans="1:22" ht="13.2" customHeight="1">
       <c r="A17" s="109"/>
-      <c r="B17" s="89"/>
-      <c r="C17" s="76">
+      <c r="B17" s="82"/>
+      <c r="C17" s="90">
         <v>43498</v>
       </c>
-      <c r="D17" s="82">
+      <c r="D17" s="84">
         <v>43641</v>
       </c>
       <c r="E17" s="54">
@@ -7239,11 +7239,11 @@
       </c>
       <c r="F17" s="53"/>
       <c r="G17" s="45"/>
-      <c r="H17" s="82">
+      <c r="H17" s="84">
         <v>43640</v>
       </c>
-      <c r="I17" s="89"/>
-      <c r="J17" s="88">
+      <c r="I17" s="82"/>
+      <c r="J17" s="81">
         <v>2</v>
       </c>
       <c r="K17" s="65"/>
@@ -7261,15 +7261,15 @@
     </row>
     <row r="18" spans="1:22" ht="13.2" customHeight="1">
       <c r="A18" s="109"/>
-      <c r="B18" s="89"/>
-      <c r="C18" s="77"/>
-      <c r="D18" s="83"/>
+      <c r="B18" s="82"/>
+      <c r="C18" s="91"/>
+      <c r="D18" s="85"/>
       <c r="E18" s="54"/>
       <c r="F18" s="53"/>
       <c r="G18" s="53"/>
-      <c r="H18" s="83"/>
-      <c r="I18" s="89"/>
-      <c r="J18" s="89"/>
+      <c r="H18" s="85"/>
+      <c r="I18" s="82"/>
+      <c r="J18" s="82"/>
       <c r="K18" s="65"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
@@ -7285,15 +7285,15 @@
     </row>
     <row r="19" spans="1:22" ht="13.2" customHeight="1">
       <c r="A19" s="109"/>
-      <c r="B19" s="89"/>
-      <c r="C19" s="77"/>
-      <c r="D19" s="83"/>
+      <c r="B19" s="82"/>
+      <c r="C19" s="91"/>
+      <c r="D19" s="85"/>
       <c r="E19" s="54"/>
       <c r="F19" s="53"/>
       <c r="G19" s="53"/>
-      <c r="H19" s="83"/>
-      <c r="I19" s="89"/>
-      <c r="J19" s="89"/>
+      <c r="H19" s="85"/>
+      <c r="I19" s="82"/>
+      <c r="J19" s="82"/>
       <c r="K19" s="65"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
@@ -7309,15 +7309,15 @@
     </row>
     <row r="20" spans="1:22" ht="13.2" customHeight="1">
       <c r="A20" s="109"/>
-      <c r="B20" s="90"/>
-      <c r="C20" s="78"/>
-      <c r="D20" s="84"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="92"/>
+      <c r="D20" s="86"/>
       <c r="E20" s="53"/>
       <c r="F20" s="53"/>
       <c r="G20" s="53"/>
-      <c r="H20" s="84"/>
-      <c r="I20" s="90"/>
-      <c r="J20" s="90"/>
+      <c r="H20" s="86"/>
+      <c r="I20" s="83"/>
+      <c r="J20" s="83"/>
       <c r="K20" s="65"/>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
@@ -7333,15 +7333,15 @@
     </row>
     <row r="21" spans="1:22" ht="13.2" customHeight="1">
       <c r="A21" s="109"/>
-      <c r="B21" s="99"/>
-      <c r="C21" s="100"/>
-      <c r="D21" s="100"/>
-      <c r="E21" s="100"/>
-      <c r="F21" s="100"/>
-      <c r="G21" s="100"/>
-      <c r="H21" s="100"/>
-      <c r="I21" s="100"/>
-      <c r="J21" s="101"/>
+      <c r="B21" s="102"/>
+      <c r="C21" s="103"/>
+      <c r="D21" s="103"/>
+      <c r="E21" s="103"/>
+      <c r="F21" s="103"/>
+      <c r="G21" s="103"/>
+      <c r="H21" s="103"/>
+      <c r="I21" s="103"/>
+      <c r="J21" s="104"/>
       <c r="K21" s="65"/>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
@@ -7357,13 +7357,13 @@
     </row>
     <row r="22" spans="1:22" ht="13.2" customHeight="1">
       <c r="A22" s="109"/>
-      <c r="B22" s="88">
+      <c r="B22" s="81">
         <v>3</v>
       </c>
-      <c r="C22" s="76">
+      <c r="C22" s="90">
         <v>43468</v>
       </c>
-      <c r="D22" s="82">
+      <c r="D22" s="84">
         <v>43645</v>
       </c>
       <c r="E22" s="54">
@@ -7371,11 +7371,11 @@
       </c>
       <c r="F22" s="27"/>
       <c r="G22" s="53"/>
-      <c r="H22" s="82"/>
-      <c r="I22" s="88">
+      <c r="H22" s="84"/>
+      <c r="I22" s="81">
         <v>4</v>
       </c>
-      <c r="J22" s="88"/>
+      <c r="J22" s="81"/>
       <c r="K22" s="65"/>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
@@ -7391,17 +7391,17 @@
     </row>
     <row r="23" spans="1:22" ht="13.2" customHeight="1">
       <c r="A23" s="109"/>
-      <c r="B23" s="89"/>
-      <c r="C23" s="77"/>
-      <c r="D23" s="83"/>
+      <c r="B23" s="82"/>
+      <c r="C23" s="91"/>
+      <c r="D23" s="85"/>
       <c r="E23" s="54">
         <v>43659</v>
       </c>
       <c r="F23" s="27"/>
       <c r="G23" s="53"/>
-      <c r="H23" s="83"/>
-      <c r="I23" s="89"/>
-      <c r="J23" s="89"/>
+      <c r="H23" s="85"/>
+      <c r="I23" s="82"/>
+      <c r="J23" s="82"/>
       <c r="K23" s="65"/>
       <c r="L23" s="10"/>
       <c r="M23" s="10"/>
@@ -7417,17 +7417,17 @@
     </row>
     <row r="24" spans="1:22" ht="13.2" customHeight="1">
       <c r="A24" s="109"/>
-      <c r="B24" s="89"/>
-      <c r="C24" s="77"/>
-      <c r="D24" s="83"/>
+      <c r="B24" s="82"/>
+      <c r="C24" s="91"/>
+      <c r="D24" s="85"/>
       <c r="E24" s="54">
-        <v>43705</v>
+        <v>43707</v>
       </c>
       <c r="F24" s="27"/>
       <c r="G24" s="53"/>
-      <c r="H24" s="83"/>
-      <c r="I24" s="89"/>
-      <c r="J24" s="89"/>
+      <c r="H24" s="85"/>
+      <c r="I24" s="82"/>
+      <c r="J24" s="82"/>
       <c r="K24" s="65"/>
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
@@ -7443,15 +7443,15 @@
     </row>
     <row r="25" spans="1:22" ht="13.2" customHeight="1">
       <c r="A25" s="109"/>
-      <c r="B25" s="89"/>
-      <c r="C25" s="78"/>
-      <c r="D25" s="84"/>
+      <c r="B25" s="82"/>
+      <c r="C25" s="92"/>
+      <c r="D25" s="86"/>
       <c r="E25" s="54"/>
       <c r="F25" s="53"/>
       <c r="G25" s="53"/>
-      <c r="H25" s="84"/>
-      <c r="I25" s="90"/>
-      <c r="J25" s="90"/>
+      <c r="H25" s="86"/>
+      <c r="I25" s="83"/>
+      <c r="J25" s="83"/>
       <c r="K25" s="65"/>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
@@ -7467,11 +7467,11 @@
     </row>
     <row r="26" spans="1:22" ht="13.2" customHeight="1">
       <c r="A26" s="109"/>
-      <c r="B26" s="89"/>
-      <c r="C26" s="76">
+      <c r="B26" s="82"/>
+      <c r="C26" s="90">
         <v>43499</v>
       </c>
-      <c r="D26" s="82">
+      <c r="D26" s="84">
         <v>43648</v>
       </c>
       <c r="E26" s="54">
@@ -7479,13 +7479,13 @@
       </c>
       <c r="F26" s="27"/>
       <c r="G26" s="53"/>
-      <c r="H26" s="82">
+      <c r="H26" s="84">
         <v>43681</v>
       </c>
-      <c r="I26" s="88">
+      <c r="I26" s="81">
         <v>3</v>
       </c>
-      <c r="J26" s="88">
+      <c r="J26" s="81">
         <v>36</v>
       </c>
       <c r="K26" s="65"/>
@@ -7503,17 +7503,17 @@
     </row>
     <row r="27" spans="1:22" ht="13.2" customHeight="1">
       <c r="A27" s="109"/>
-      <c r="B27" s="89"/>
-      <c r="C27" s="77"/>
-      <c r="D27" s="83"/>
+      <c r="B27" s="82"/>
+      <c r="C27" s="91"/>
+      <c r="D27" s="85"/>
       <c r="E27" s="54">
         <v>43661</v>
       </c>
       <c r="F27" s="27"/>
       <c r="G27" s="53"/>
-      <c r="H27" s="83"/>
-      <c r="I27" s="89"/>
-      <c r="J27" s="89"/>
+      <c r="H27" s="85"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="82"/>
       <c r="K27" s="65"/>
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
@@ -7529,17 +7529,17 @@
     </row>
     <row r="28" spans="1:22" ht="13.2" customHeight="1">
       <c r="A28" s="109"/>
-      <c r="B28" s="89"/>
-      <c r="C28" s="77"/>
-      <c r="D28" s="83"/>
+      <c r="B28" s="82"/>
+      <c r="C28" s="91"/>
+      <c r="D28" s="85"/>
       <c r="E28" s="54">
         <v>43681</v>
       </c>
       <c r="F28" s="44"/>
       <c r="G28" s="45"/>
-      <c r="H28" s="83"/>
-      <c r="I28" s="89"/>
-      <c r="J28" s="89"/>
+      <c r="H28" s="85"/>
+      <c r="I28" s="82"/>
+      <c r="J28" s="82"/>
       <c r="K28" s="65"/>
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
@@ -7555,15 +7555,15 @@
     </row>
     <row r="29" spans="1:22" ht="13.2" customHeight="1">
       <c r="A29" s="110"/>
-      <c r="B29" s="90"/>
-      <c r="C29" s="78"/>
-      <c r="D29" s="84"/>
+      <c r="B29" s="83"/>
+      <c r="C29" s="92"/>
+      <c r="D29" s="86"/>
       <c r="E29" s="53"/>
       <c r="F29" s="53"/>
       <c r="G29" s="53"/>
-      <c r="H29" s="84"/>
-      <c r="I29" s="90"/>
-      <c r="J29" s="90"/>
+      <c r="H29" s="86"/>
+      <c r="I29" s="83"/>
+      <c r="J29" s="83"/>
       <c r="K29" s="65"/>
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
@@ -7605,13 +7605,13 @@
       <c r="A31" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="88">
+      <c r="B31" s="81">
         <v>1</v>
       </c>
-      <c r="C31" s="88" t="s">
+      <c r="C31" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="82">
+      <c r="D31" s="84">
         <v>43654</v>
       </c>
       <c r="E31" s="54">
@@ -7619,13 +7619,13 @@
       </c>
       <c r="F31" s="27"/>
       <c r="G31" s="53"/>
-      <c r="H31" s="82">
+      <c r="H31" s="84">
         <v>43660</v>
       </c>
-      <c r="I31" s="88">
+      <c r="I31" s="81">
         <v>6</v>
       </c>
-      <c r="J31" s="88">
+      <c r="J31" s="81">
         <v>12</v>
       </c>
       <c r="K31" s="65"/>
@@ -7633,127 +7633,127 @@
     </row>
     <row r="32" spans="1:22" ht="13.2" customHeight="1">
       <c r="A32" s="109"/>
-      <c r="B32" s="89"/>
-      <c r="C32" s="89"/>
-      <c r="D32" s="83"/>
+      <c r="B32" s="82"/>
+      <c r="C32" s="82"/>
+      <c r="D32" s="85"/>
       <c r="E32" s="54">
         <v>43660</v>
       </c>
       <c r="F32" s="53"/>
       <c r="G32" s="26"/>
-      <c r="H32" s="83"/>
-      <c r="I32" s="89"/>
-      <c r="J32" s="89"/>
+      <c r="H32" s="85"/>
+      <c r="I32" s="82"/>
+      <c r="J32" s="82"/>
       <c r="K32" s="65"/>
       <c r="V32" s="10"/>
     </row>
     <row r="33" spans="1:22" ht="13.2" customHeight="1">
       <c r="A33" s="109"/>
-      <c r="B33" s="89"/>
-      <c r="C33" s="89"/>
-      <c r="D33" s="83"/>
+      <c r="B33" s="82"/>
+      <c r="C33" s="82"/>
+      <c r="D33" s="85"/>
       <c r="E33" s="54"/>
       <c r="F33" s="53"/>
       <c r="G33" s="53"/>
-      <c r="H33" s="83"/>
-      <c r="I33" s="89"/>
-      <c r="J33" s="89"/>
+      <c r="H33" s="85"/>
+      <c r="I33" s="82"/>
+      <c r="J33" s="82"/>
       <c r="K33" s="65"/>
       <c r="V33" s="10"/>
     </row>
     <row r="34" spans="1:22" ht="13.2" customHeight="1">
       <c r="A34" s="109"/>
-      <c r="B34" s="89"/>
-      <c r="C34" s="89"/>
-      <c r="D34" s="83"/>
+      <c r="B34" s="82"/>
+      <c r="C34" s="82"/>
+      <c r="D34" s="85"/>
       <c r="E34" s="54"/>
       <c r="F34" s="53"/>
       <c r="G34" s="53"/>
-      <c r="H34" s="83"/>
-      <c r="I34" s="89"/>
-      <c r="J34" s="89"/>
+      <c r="H34" s="85"/>
+      <c r="I34" s="82"/>
+      <c r="J34" s="82"/>
       <c r="K34" s="65"/>
       <c r="V34" s="10"/>
     </row>
     <row r="35" spans="1:22" ht="13.2" customHeight="1">
       <c r="A35" s="109"/>
-      <c r="B35" s="89"/>
-      <c r="C35" s="89"/>
-      <c r="D35" s="83"/>
+      <c r="B35" s="82"/>
+      <c r="C35" s="82"/>
+      <c r="D35" s="85"/>
       <c r="E35" s="54"/>
       <c r="F35" s="53"/>
       <c r="G35" s="53"/>
-      <c r="H35" s="83"/>
-      <c r="I35" s="89"/>
-      <c r="J35" s="89"/>
+      <c r="H35" s="85"/>
+      <c r="I35" s="82"/>
+      <c r="J35" s="82"/>
       <c r="K35" s="65"/>
       <c r="V35" s="10"/>
     </row>
     <row r="36" spans="1:22" ht="13.2" customHeight="1">
       <c r="A36" s="109"/>
-      <c r="B36" s="89"/>
-      <c r="C36" s="89"/>
-      <c r="D36" s="83"/>
+      <c r="B36" s="82"/>
+      <c r="C36" s="82"/>
+      <c r="D36" s="85"/>
       <c r="E36" s="53"/>
       <c r="F36" s="53"/>
       <c r="G36" s="53"/>
-      <c r="H36" s="83"/>
-      <c r="I36" s="89"/>
-      <c r="J36" s="89"/>
+      <c r="H36" s="85"/>
+      <c r="I36" s="82"/>
+      <c r="J36" s="82"/>
       <c r="K36" s="65"/>
       <c r="V36" s="10"/>
     </row>
     <row r="37" spans="1:22" ht="13.2" customHeight="1">
       <c r="A37" s="109"/>
-      <c r="B37" s="89"/>
-      <c r="C37" s="89"/>
-      <c r="D37" s="83"/>
+      <c r="B37" s="82"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="85"/>
       <c r="E37" s="53"/>
       <c r="F37" s="53"/>
       <c r="G37" s="53"/>
-      <c r="H37" s="83"/>
-      <c r="I37" s="89"/>
-      <c r="J37" s="89"/>
+      <c r="H37" s="85"/>
+      <c r="I37" s="82"/>
+      <c r="J37" s="82"/>
       <c r="K37" s="65"/>
       <c r="V37" s="10"/>
     </row>
     <row r="38" spans="1:22" ht="13.2" customHeight="1">
       <c r="A38" s="109"/>
-      <c r="B38" s="90"/>
-      <c r="C38" s="90"/>
-      <c r="D38" s="84"/>
+      <c r="B38" s="83"/>
+      <c r="C38" s="83"/>
+      <c r="D38" s="86"/>
       <c r="E38" s="53"/>
       <c r="F38" s="53"/>
       <c r="G38" s="53"/>
-      <c r="H38" s="84"/>
-      <c r="I38" s="90"/>
-      <c r="J38" s="90"/>
+      <c r="H38" s="86"/>
+      <c r="I38" s="83"/>
+      <c r="J38" s="83"/>
       <c r="K38" s="65"/>
       <c r="V38" s="10"/>
     </row>
     <row r="39" spans="1:22" ht="13.2" customHeight="1">
       <c r="A39" s="109"/>
-      <c r="B39" s="85"/>
-      <c r="C39" s="86"/>
-      <c r="D39" s="86"/>
-      <c r="E39" s="86"/>
-      <c r="F39" s="86"/>
-      <c r="G39" s="86"/>
-      <c r="H39" s="86"/>
-      <c r="I39" s="86"/>
-      <c r="J39" s="87"/>
+      <c r="B39" s="78"/>
+      <c r="C39" s="79"/>
+      <c r="D39" s="79"/>
+      <c r="E39" s="79"/>
+      <c r="F39" s="79"/>
+      <c r="G39" s="79"/>
+      <c r="H39" s="79"/>
+      <c r="I39" s="79"/>
+      <c r="J39" s="80"/>
       <c r="K39" s="65"/>
       <c r="V39" s="10"/>
     </row>
     <row r="40" spans="1:22" ht="13.2" customHeight="1">
       <c r="A40" s="109"/>
-      <c r="B40" s="88">
+      <c r="B40" s="81">
         <v>2</v>
       </c>
-      <c r="C40" s="76">
+      <c r="C40" s="90">
         <v>43467</v>
       </c>
-      <c r="D40" s="82">
+      <c r="D40" s="84">
         <v>43657</v>
       </c>
       <c r="E40" s="54">
@@ -7764,10 +7764,10 @@
       <c r="H40" s="148">
         <v>43675</v>
       </c>
-      <c r="I40" s="88">
+      <c r="I40" s="81">
         <v>3</v>
       </c>
-      <c r="J40" s="88">
+      <c r="J40" s="81">
         <v>21</v>
       </c>
       <c r="K40" s="65"/>
@@ -7775,57 +7775,57 @@
     </row>
     <row r="41" spans="1:22" ht="13.2" customHeight="1">
       <c r="A41" s="109"/>
-      <c r="B41" s="89"/>
-      <c r="C41" s="77"/>
-      <c r="D41" s="83"/>
+      <c r="B41" s="82"/>
+      <c r="C41" s="91"/>
+      <c r="D41" s="85"/>
       <c r="E41" s="54">
         <v>43665</v>
       </c>
       <c r="F41" s="42"/>
       <c r="G41" s="51"/>
       <c r="H41" s="149"/>
-      <c r="I41" s="89"/>
-      <c r="J41" s="89"/>
+      <c r="I41" s="82"/>
+      <c r="J41" s="82"/>
       <c r="K41" s="65"/>
       <c r="V41" s="10"/>
     </row>
     <row r="42" spans="1:22" ht="13.2" customHeight="1">
       <c r="A42" s="109"/>
-      <c r="B42" s="89"/>
-      <c r="C42" s="77"/>
-      <c r="D42" s="83"/>
+      <c r="B42" s="82"/>
+      <c r="C42" s="91"/>
+      <c r="D42" s="85"/>
       <c r="E42" s="41">
         <v>43675</v>
       </c>
       <c r="F42" s="51"/>
       <c r="G42" s="45"/>
       <c r="H42" s="149"/>
-      <c r="I42" s="89"/>
-      <c r="J42" s="89"/>
+      <c r="I42" s="82"/>
+      <c r="J42" s="82"/>
       <c r="K42" s="65"/>
       <c r="V42" s="10"/>
     </row>
     <row r="43" spans="1:22" ht="13.2" customHeight="1">
       <c r="A43" s="109"/>
-      <c r="B43" s="89"/>
-      <c r="C43" s="78"/>
-      <c r="D43" s="84"/>
+      <c r="B43" s="82"/>
+      <c r="C43" s="92"/>
+      <c r="D43" s="86"/>
       <c r="E43" s="54"/>
       <c r="F43" s="53"/>
       <c r="G43" s="53"/>
       <c r="H43" s="150"/>
-      <c r="I43" s="89"/>
-      <c r="J43" s="90"/>
+      <c r="I43" s="82"/>
+      <c r="J43" s="83"/>
       <c r="K43" s="65"/>
       <c r="V43" s="10"/>
     </row>
     <row r="44" spans="1:22" ht="13.2" customHeight="1">
       <c r="A44" s="109"/>
-      <c r="B44" s="89"/>
-      <c r="C44" s="76">
+      <c r="B44" s="82"/>
+      <c r="C44" s="90">
         <v>43498</v>
       </c>
-      <c r="D44" s="82">
+      <c r="D44" s="84">
         <v>43657</v>
       </c>
       <c r="E44" s="54">
@@ -7836,8 +7836,8 @@
       <c r="H44" s="148">
         <v>43675</v>
       </c>
-      <c r="I44" s="89"/>
-      <c r="J44" s="88">
+      <c r="I44" s="82"/>
+      <c r="J44" s="81">
         <v>21</v>
       </c>
       <c r="K44" s="65"/>
@@ -7845,73 +7845,73 @@
     </row>
     <row r="45" spans="1:22" ht="13.2" customHeight="1">
       <c r="A45" s="109"/>
-      <c r="B45" s="89"/>
-      <c r="C45" s="77"/>
-      <c r="D45" s="83"/>
+      <c r="B45" s="82"/>
+      <c r="C45" s="91"/>
+      <c r="D45" s="85"/>
       <c r="E45" s="54">
         <v>43665</v>
       </c>
       <c r="F45" s="42"/>
       <c r="G45" s="51"/>
       <c r="H45" s="149"/>
-      <c r="I45" s="89"/>
-      <c r="J45" s="89"/>
+      <c r="I45" s="82"/>
+      <c r="J45" s="82"/>
       <c r="K45" s="65"/>
       <c r="V45" s="10"/>
     </row>
     <row r="46" spans="1:22" ht="13.2" customHeight="1">
       <c r="A46" s="109"/>
-      <c r="B46" s="89"/>
-      <c r="C46" s="77"/>
-      <c r="D46" s="83"/>
+      <c r="B46" s="82"/>
+      <c r="C46" s="91"/>
+      <c r="D46" s="85"/>
       <c r="E46" s="41">
         <v>43675</v>
       </c>
       <c r="F46" s="51"/>
       <c r="G46" s="45"/>
       <c r="H46" s="149"/>
-      <c r="I46" s="89"/>
-      <c r="J46" s="89"/>
+      <c r="I46" s="82"/>
+      <c r="J46" s="82"/>
       <c r="K46" s="65"/>
       <c r="V46" s="10"/>
     </row>
     <row r="47" spans="1:22" ht="13.2" customHeight="1">
       <c r="A47" s="109"/>
-      <c r="B47" s="90"/>
-      <c r="C47" s="78"/>
-      <c r="D47" s="84"/>
+      <c r="B47" s="83"/>
+      <c r="C47" s="92"/>
+      <c r="D47" s="86"/>
       <c r="E47" s="53"/>
       <c r="F47" s="53"/>
       <c r="G47" s="53"/>
       <c r="H47" s="150"/>
-      <c r="I47" s="90"/>
-      <c r="J47" s="90"/>
+      <c r="I47" s="83"/>
+      <c r="J47" s="83"/>
       <c r="K47" s="65"/>
       <c r="V47" s="10"/>
     </row>
     <row r="48" spans="1:22" ht="13.2" customHeight="1">
       <c r="A48" s="109"/>
-      <c r="B48" s="99"/>
-      <c r="C48" s="100"/>
-      <c r="D48" s="100"/>
-      <c r="E48" s="100"/>
-      <c r="F48" s="100"/>
-      <c r="G48" s="100"/>
-      <c r="H48" s="100"/>
-      <c r="I48" s="100"/>
-      <c r="J48" s="101"/>
+      <c r="B48" s="102"/>
+      <c r="C48" s="103"/>
+      <c r="D48" s="103"/>
+      <c r="E48" s="103"/>
+      <c r="F48" s="103"/>
+      <c r="G48" s="103"/>
+      <c r="H48" s="103"/>
+      <c r="I48" s="103"/>
+      <c r="J48" s="104"/>
       <c r="K48" s="65"/>
       <c r="V48" s="10"/>
     </row>
     <row r="49" spans="1:22" ht="13.2" customHeight="1">
       <c r="A49" s="109"/>
-      <c r="B49" s="88">
+      <c r="B49" s="81">
         <v>3</v>
       </c>
-      <c r="C49" s="76">
+      <c r="C49" s="90">
         <v>43468</v>
       </c>
-      <c r="D49" s="82">
+      <c r="D49" s="84">
         <v>43661</v>
       </c>
       <c r="E49" s="54">
@@ -7919,67 +7919,67 @@
       </c>
       <c r="F49" s="27"/>
       <c r="G49" s="53"/>
-      <c r="H49" s="82"/>
-      <c r="I49" s="88">
+      <c r="H49" s="84"/>
+      <c r="I49" s="81">
         <v>4</v>
       </c>
-      <c r="J49" s="88"/>
+      <c r="J49" s="81"/>
       <c r="K49" s="65"/>
       <c r="V49" s="10"/>
     </row>
     <row r="50" spans="1:22" ht="13.2" customHeight="1">
       <c r="A50" s="109"/>
-      <c r="B50" s="89"/>
-      <c r="C50" s="77"/>
-      <c r="D50" s="83"/>
+      <c r="B50" s="82"/>
+      <c r="C50" s="91"/>
+      <c r="D50" s="85"/>
       <c r="E50" s="54">
         <v>43672</v>
       </c>
       <c r="F50" s="27"/>
       <c r="G50" s="53"/>
-      <c r="H50" s="83"/>
-      <c r="I50" s="89"/>
-      <c r="J50" s="89"/>
+      <c r="H50" s="85"/>
+      <c r="I50" s="82"/>
+      <c r="J50" s="82"/>
       <c r="K50" s="65"/>
       <c r="V50" s="10"/>
     </row>
     <row r="51" spans="1:22" ht="13.2" customHeight="1">
       <c r="A51" s="109"/>
-      <c r="B51" s="89"/>
-      <c r="C51" s="77"/>
-      <c r="D51" s="83"/>
+      <c r="B51" s="82"/>
+      <c r="C51" s="91"/>
+      <c r="D51" s="85"/>
       <c r="E51" s="54">
-        <v>43705</v>
+        <v>43707</v>
       </c>
       <c r="F51" s="27"/>
       <c r="G51" s="53"/>
-      <c r="H51" s="83"/>
-      <c r="I51" s="89"/>
-      <c r="J51" s="89"/>
+      <c r="H51" s="85"/>
+      <c r="I51" s="82"/>
+      <c r="J51" s="82"/>
       <c r="K51" s="65"/>
       <c r="V51" s="10"/>
     </row>
     <row r="52" spans="1:22" ht="13.2" customHeight="1">
       <c r="A52" s="109"/>
-      <c r="B52" s="89"/>
-      <c r="C52" s="78"/>
-      <c r="D52" s="84"/>
+      <c r="B52" s="82"/>
+      <c r="C52" s="92"/>
+      <c r="D52" s="86"/>
       <c r="E52" s="53"/>
       <c r="F52" s="53"/>
       <c r="G52" s="53"/>
-      <c r="H52" s="84"/>
-      <c r="I52" s="90"/>
-      <c r="J52" s="90"/>
+      <c r="H52" s="86"/>
+      <c r="I52" s="83"/>
+      <c r="J52" s="83"/>
       <c r="K52" s="65"/>
       <c r="V52" s="10"/>
     </row>
     <row r="53" spans="1:22" ht="13.2" customHeight="1">
       <c r="A53" s="109"/>
-      <c r="B53" s="89"/>
-      <c r="C53" s="76">
+      <c r="B53" s="82"/>
+      <c r="C53" s="90">
         <v>43499</v>
       </c>
-      <c r="D53" s="82">
+      <c r="D53" s="84">
         <v>43664</v>
       </c>
       <c r="E53" s="54">
@@ -7987,13 +7987,13 @@
       </c>
       <c r="F53" s="27"/>
       <c r="G53" s="53"/>
-      <c r="H53" s="82">
+      <c r="H53" s="84">
         <v>43675</v>
       </c>
-      <c r="I53" s="102">
+      <c r="I53" s="105">
         <v>3</v>
       </c>
-      <c r="J53" s="88">
+      <c r="J53" s="81">
         <v>14</v>
       </c>
       <c r="K53" s="65"/>
@@ -8001,59 +8001,59 @@
     </row>
     <row r="54" spans="1:22" ht="13.2" customHeight="1">
       <c r="A54" s="109"/>
-      <c r="B54" s="89"/>
-      <c r="C54" s="77"/>
-      <c r="D54" s="83"/>
+      <c r="B54" s="82"/>
+      <c r="C54" s="91"/>
+      <c r="D54" s="85"/>
       <c r="E54" s="54">
         <v>43675</v>
       </c>
       <c r="F54" s="44"/>
       <c r="G54" s="45"/>
-      <c r="H54" s="83"/>
-      <c r="I54" s="103"/>
-      <c r="J54" s="89"/>
+      <c r="H54" s="85"/>
+      <c r="I54" s="106"/>
+      <c r="J54" s="82"/>
       <c r="K54" s="65"/>
       <c r="V54" s="10"/>
     </row>
     <row r="55" spans="1:22" ht="13.2" customHeight="1">
       <c r="A55" s="109"/>
-      <c r="B55" s="89"/>
-      <c r="C55" s="77"/>
-      <c r="D55" s="83"/>
+      <c r="B55" s="82"/>
+      <c r="C55" s="91"/>
+      <c r="D55" s="85"/>
       <c r="E55" s="53"/>
       <c r="F55" s="53"/>
       <c r="G55" s="53"/>
-      <c r="H55" s="83"/>
-      <c r="I55" s="103"/>
-      <c r="J55" s="89"/>
+      <c r="H55" s="85"/>
+      <c r="I55" s="106"/>
+      <c r="J55" s="82"/>
       <c r="K55" s="65"/>
       <c r="V55" s="10"/>
     </row>
     <row r="56" spans="1:22" ht="13.2" customHeight="1">
       <c r="A56" s="110"/>
-      <c r="B56" s="90"/>
-      <c r="C56" s="78"/>
-      <c r="D56" s="84"/>
+      <c r="B56" s="83"/>
+      <c r="C56" s="92"/>
+      <c r="D56" s="86"/>
       <c r="E56" s="53"/>
       <c r="F56" s="53"/>
       <c r="G56" s="53"/>
-      <c r="H56" s="84"/>
-      <c r="I56" s="104"/>
-      <c r="J56" s="90"/>
+      <c r="H56" s="86"/>
+      <c r="I56" s="107"/>
+      <c r="J56" s="83"/>
       <c r="K56" s="65"/>
       <c r="V56" s="10"/>
     </row>
     <row r="57" spans="1:22" ht="13.2" customHeight="1">
-      <c r="A57" s="96"/>
-      <c r="B57" s="97"/>
-      <c r="C57" s="97"/>
-      <c r="D57" s="97"/>
-      <c r="E57" s="97"/>
-      <c r="F57" s="97"/>
-      <c r="G57" s="97"/>
-      <c r="H57" s="97"/>
-      <c r="I57" s="97"/>
-      <c r="J57" s="98"/>
+      <c r="A57" s="99"/>
+      <c r="B57" s="100"/>
+      <c r="C57" s="100"/>
+      <c r="D57" s="100"/>
+      <c r="E57" s="100"/>
+      <c r="F57" s="100"/>
+      <c r="G57" s="100"/>
+      <c r="H57" s="100"/>
+      <c r="I57" s="100"/>
+      <c r="J57" s="101"/>
       <c r="K57" s="65"/>
       <c r="V57" s="10"/>
     </row>
@@ -8061,13 +8061,13 @@
       <c r="A58" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="B58" s="88">
+      <c r="B58" s="81">
         <v>1</v>
       </c>
-      <c r="C58" s="88" t="s">
+      <c r="C58" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="D58" s="82">
+      <c r="D58" s="84">
         <v>43670</v>
       </c>
       <c r="E58" s="48">
@@ -8075,13 +8075,13 @@
       </c>
       <c r="F58" s="49"/>
       <c r="G58" s="53"/>
-      <c r="H58" s="82">
+      <c r="H58" s="84">
         <v>43678</v>
       </c>
-      <c r="I58" s="88">
+      <c r="I58" s="81">
         <v>6</v>
       </c>
-      <c r="J58" s="88">
+      <c r="J58" s="81">
         <v>14</v>
       </c>
       <c r="K58" s="65"/>
@@ -8099,17 +8099,17 @@
     </row>
     <row r="59" spans="1:22" ht="13.2" customHeight="1">
       <c r="A59" s="109"/>
-      <c r="B59" s="89"/>
-      <c r="C59" s="89"/>
-      <c r="D59" s="83"/>
+      <c r="B59" s="82"/>
+      <c r="C59" s="82"/>
+      <c r="D59" s="85"/>
       <c r="E59" s="74">
         <v>43674</v>
       </c>
       <c r="F59" s="75"/>
       <c r="G59" s="57"/>
-      <c r="H59" s="83"/>
-      <c r="I59" s="89"/>
-      <c r="J59" s="89"/>
+      <c r="H59" s="85"/>
+      <c r="I59" s="82"/>
+      <c r="J59" s="82"/>
       <c r="K59" s="65"/>
       <c r="L59" s="10"/>
       <c r="M59" s="10"/>
@@ -8125,17 +8125,17 @@
     </row>
     <row r="60" spans="1:22" ht="13.2" customHeight="1">
       <c r="A60" s="109"/>
-      <c r="B60" s="89"/>
-      <c r="C60" s="89"/>
-      <c r="D60" s="83"/>
+      <c r="B60" s="82"/>
+      <c r="C60" s="82"/>
+      <c r="D60" s="85"/>
       <c r="E60" s="48">
         <v>43679</v>
       </c>
       <c r="F60" s="53"/>
       <c r="G60" s="45"/>
-      <c r="H60" s="83"/>
-      <c r="I60" s="89"/>
-      <c r="J60" s="89"/>
+      <c r="H60" s="85"/>
+      <c r="I60" s="82"/>
+      <c r="J60" s="82"/>
       <c r="K60" s="65"/>
       <c r="L60" s="10"/>
       <c r="M60" s="10"/>
@@ -8151,15 +8151,15 @@
     </row>
     <row r="61" spans="1:22" ht="13.2" customHeight="1">
       <c r="A61" s="109"/>
-      <c r="B61" s="89"/>
-      <c r="C61" s="89"/>
-      <c r="D61" s="83"/>
+      <c r="B61" s="82"/>
+      <c r="C61" s="82"/>
+      <c r="D61" s="85"/>
       <c r="E61" s="71"/>
       <c r="F61" s="71"/>
       <c r="G61" s="71"/>
-      <c r="H61" s="83"/>
-      <c r="I61" s="89"/>
-      <c r="J61" s="89"/>
+      <c r="H61" s="85"/>
+      <c r="I61" s="82"/>
+      <c r="J61" s="82"/>
       <c r="K61" s="65"/>
       <c r="L61" s="10"/>
       <c r="M61" s="10"/>
@@ -8175,88 +8175,88 @@
     </row>
     <row r="62" spans="1:22" ht="13.2" customHeight="1">
       <c r="A62" s="109"/>
-      <c r="B62" s="89"/>
-      <c r="C62" s="89"/>
-      <c r="D62" s="83"/>
+      <c r="B62" s="82"/>
+      <c r="C62" s="82"/>
+      <c r="D62" s="85"/>
       <c r="E62" s="72"/>
       <c r="F62" s="72"/>
       <c r="G62" s="72"/>
-      <c r="H62" s="83"/>
-      <c r="I62" s="89"/>
-      <c r="J62" s="89"/>
+      <c r="H62" s="85"/>
+      <c r="I62" s="82"/>
+      <c r="J62" s="82"/>
       <c r="K62" s="65"/>
       <c r="U62" s="10"/>
       <c r="V62" s="10"/>
     </row>
     <row r="63" spans="1:22" ht="13.2" customHeight="1">
       <c r="A63" s="109"/>
-      <c r="B63" s="89"/>
-      <c r="C63" s="89"/>
-      <c r="D63" s="83"/>
+      <c r="B63" s="82"/>
+      <c r="C63" s="82"/>
+      <c r="D63" s="85"/>
       <c r="E63" s="71"/>
       <c r="F63" s="71"/>
       <c r="G63" s="71"/>
-      <c r="H63" s="83"/>
-      <c r="I63" s="89"/>
-      <c r="J63" s="89"/>
+      <c r="H63" s="85"/>
+      <c r="I63" s="82"/>
+      <c r="J63" s="82"/>
       <c r="K63" s="65"/>
       <c r="U63" s="10"/>
       <c r="V63" s="10"/>
     </row>
     <row r="64" spans="1:22" ht="13.2" customHeight="1">
       <c r="A64" s="109"/>
-      <c r="B64" s="89"/>
-      <c r="C64" s="89"/>
-      <c r="D64" s="83"/>
+      <c r="B64" s="82"/>
+      <c r="C64" s="82"/>
+      <c r="D64" s="85"/>
       <c r="E64" s="53"/>
       <c r="F64" s="53"/>
       <c r="G64" s="53"/>
-      <c r="H64" s="83"/>
-      <c r="I64" s="89"/>
-      <c r="J64" s="89"/>
+      <c r="H64" s="85"/>
+      <c r="I64" s="82"/>
+      <c r="J64" s="82"/>
       <c r="K64" s="65"/>
       <c r="U64" s="10"/>
       <c r="V64" s="10"/>
     </row>
     <row r="65" spans="1:22" ht="13.2" customHeight="1">
       <c r="A65" s="109"/>
-      <c r="B65" s="90"/>
-      <c r="C65" s="90"/>
-      <c r="D65" s="84"/>
+      <c r="B65" s="83"/>
+      <c r="C65" s="83"/>
+      <c r="D65" s="86"/>
       <c r="E65" s="53"/>
       <c r="F65" s="53"/>
       <c r="G65" s="53"/>
-      <c r="H65" s="84"/>
-      <c r="I65" s="90"/>
-      <c r="J65" s="90"/>
+      <c r="H65" s="86"/>
+      <c r="I65" s="83"/>
+      <c r="J65" s="83"/>
       <c r="K65" s="65"/>
       <c r="U65" s="10"/>
       <c r="V65" s="10"/>
     </row>
     <row r="66" spans="1:22" ht="13.2" customHeight="1">
       <c r="A66" s="109"/>
-      <c r="B66" s="85"/>
-      <c r="C66" s="86"/>
-      <c r="D66" s="86"/>
-      <c r="E66" s="86"/>
-      <c r="F66" s="86"/>
-      <c r="G66" s="86"/>
-      <c r="H66" s="86"/>
-      <c r="I66" s="86"/>
-      <c r="J66" s="87"/>
+      <c r="B66" s="78"/>
+      <c r="C66" s="79"/>
+      <c r="D66" s="79"/>
+      <c r="E66" s="79"/>
+      <c r="F66" s="79"/>
+      <c r="G66" s="79"/>
+      <c r="H66" s="79"/>
+      <c r="I66" s="79"/>
+      <c r="J66" s="80"/>
       <c r="K66" s="65"/>
       <c r="U66" s="10"/>
       <c r="V66" s="10"/>
     </row>
     <row r="67" spans="1:22" ht="13.2" customHeight="1">
       <c r="A67" s="109"/>
-      <c r="B67" s="88">
+      <c r="B67" s="81">
         <v>2</v>
       </c>
-      <c r="C67" s="76">
+      <c r="C67" s="90">
         <v>43467</v>
       </c>
-      <c r="D67" s="82">
+      <c r="D67" s="84">
         <v>43673</v>
       </c>
       <c r="E67" s="48">
@@ -8264,13 +8264,13 @@
       </c>
       <c r="F67" s="46"/>
       <c r="G67" s="53"/>
-      <c r="H67" s="82">
+      <c r="H67" s="84">
         <v>43678</v>
       </c>
-      <c r="I67" s="88">
+      <c r="I67" s="81">
         <v>3</v>
       </c>
-      <c r="J67" s="88">
+      <c r="J67" s="81">
         <v>8</v>
       </c>
       <c r="K67" s="65"/>
@@ -8279,60 +8279,60 @@
     </row>
     <row r="68" spans="1:22" ht="13.2" customHeight="1">
       <c r="A68" s="109"/>
-      <c r="B68" s="89"/>
-      <c r="C68" s="77"/>
-      <c r="D68" s="83"/>
+      <c r="B68" s="82"/>
+      <c r="C68" s="91"/>
+      <c r="D68" s="85"/>
       <c r="E68" s="48">
         <v>43674</v>
       </c>
       <c r="F68" s="49"/>
       <c r="G68" s="57"/>
-      <c r="H68" s="83"/>
-      <c r="I68" s="89"/>
-      <c r="J68" s="89"/>
+      <c r="H68" s="85"/>
+      <c r="I68" s="82"/>
+      <c r="J68" s="82"/>
       <c r="K68" s="65"/>
       <c r="U68" s="10"/>
       <c r="V68" s="10"/>
     </row>
     <row r="69" spans="1:22" ht="13.2" customHeight="1">
       <c r="A69" s="109"/>
-      <c r="B69" s="89"/>
-      <c r="C69" s="77"/>
-      <c r="D69" s="83"/>
+      <c r="B69" s="82"/>
+      <c r="C69" s="91"/>
+      <c r="D69" s="85"/>
       <c r="E69" s="48">
         <v>43679</v>
       </c>
       <c r="F69" s="53"/>
       <c r="G69" s="45"/>
-      <c r="H69" s="83"/>
-      <c r="I69" s="89"/>
-      <c r="J69" s="89"/>
+      <c r="H69" s="85"/>
+      <c r="I69" s="82"/>
+      <c r="J69" s="82"/>
       <c r="K69" s="65"/>
       <c r="U69" s="10"/>
       <c r="V69" s="10"/>
     </row>
     <row r="70" spans="1:22" ht="13.2" customHeight="1">
       <c r="A70" s="109"/>
-      <c r="B70" s="89"/>
-      <c r="C70" s="78"/>
-      <c r="D70" s="84"/>
+      <c r="B70" s="82"/>
+      <c r="C70" s="92"/>
+      <c r="D70" s="86"/>
       <c r="E70" s="53"/>
       <c r="F70" s="53"/>
       <c r="G70" s="53"/>
-      <c r="H70" s="84"/>
-      <c r="I70" s="89"/>
-      <c r="J70" s="90"/>
+      <c r="H70" s="86"/>
+      <c r="I70" s="82"/>
+      <c r="J70" s="83"/>
       <c r="K70" s="65"/>
       <c r="U70" s="10"/>
       <c r="V70" s="10"/>
     </row>
     <row r="71" spans="1:22" ht="13.2" customHeight="1">
       <c r="A71" s="109"/>
-      <c r="B71" s="89"/>
-      <c r="C71" s="76">
+      <c r="B71" s="82"/>
+      <c r="C71" s="90">
         <v>43498</v>
       </c>
-      <c r="D71" s="82">
+      <c r="D71" s="84">
         <v>43673</v>
       </c>
       <c r="E71" s="48">
@@ -8340,11 +8340,11 @@
       </c>
       <c r="F71" s="49"/>
       <c r="G71" s="53"/>
-      <c r="H71" s="82">
+      <c r="H71" s="84">
         <v>43678</v>
       </c>
-      <c r="I71" s="89"/>
-      <c r="J71" s="88">
+      <c r="I71" s="82"/>
+      <c r="J71" s="81">
         <v>8</v>
       </c>
       <c r="K71" s="65"/>
@@ -8353,77 +8353,77 @@
     </row>
     <row r="72" spans="1:22" ht="13.2" customHeight="1">
       <c r="A72" s="109"/>
-      <c r="B72" s="89"/>
-      <c r="C72" s="77"/>
-      <c r="D72" s="83"/>
+      <c r="B72" s="82"/>
+      <c r="C72" s="91"/>
+      <c r="D72" s="85"/>
       <c r="E72" s="48">
         <v>43674</v>
       </c>
       <c r="F72" s="49"/>
       <c r="G72" s="44"/>
-      <c r="H72" s="83"/>
-      <c r="I72" s="89"/>
-      <c r="J72" s="89"/>
+      <c r="H72" s="85"/>
+      <c r="I72" s="82"/>
+      <c r="J72" s="82"/>
       <c r="K72" s="65"/>
       <c r="U72" s="10"/>
       <c r="V72" s="10"/>
     </row>
     <row r="73" spans="1:22" ht="13.2" customHeight="1">
       <c r="A73" s="109"/>
-      <c r="B73" s="89"/>
-      <c r="C73" s="77"/>
-      <c r="D73" s="83"/>
+      <c r="B73" s="82"/>
+      <c r="C73" s="91"/>
+      <c r="D73" s="85"/>
       <c r="E73" s="48">
         <v>43679</v>
       </c>
       <c r="F73" s="53"/>
       <c r="G73" s="45"/>
-      <c r="H73" s="83"/>
-      <c r="I73" s="89"/>
-      <c r="J73" s="89"/>
+      <c r="H73" s="85"/>
+      <c r="I73" s="82"/>
+      <c r="J73" s="82"/>
       <c r="K73" s="65"/>
       <c r="U73" s="10"/>
       <c r="V73" s="10"/>
     </row>
     <row r="74" spans="1:22" ht="13.2" customHeight="1">
       <c r="A74" s="109"/>
-      <c r="B74" s="90"/>
-      <c r="C74" s="78"/>
-      <c r="D74" s="84"/>
+      <c r="B74" s="83"/>
+      <c r="C74" s="92"/>
+      <c r="D74" s="86"/>
       <c r="E74" s="53"/>
       <c r="F74" s="53"/>
       <c r="G74" s="53"/>
-      <c r="H74" s="84"/>
-      <c r="I74" s="90"/>
-      <c r="J74" s="90"/>
+      <c r="H74" s="86"/>
+      <c r="I74" s="83"/>
+      <c r="J74" s="83"/>
       <c r="K74" s="65"/>
       <c r="U74" s="10"/>
       <c r="V74" s="10"/>
     </row>
     <row r="75" spans="1:22" ht="13.2" customHeight="1">
       <c r="A75" s="109"/>
-      <c r="B75" s="99"/>
-      <c r="C75" s="100"/>
-      <c r="D75" s="100"/>
-      <c r="E75" s="100"/>
-      <c r="F75" s="100"/>
-      <c r="G75" s="100"/>
-      <c r="H75" s="100"/>
-      <c r="I75" s="100"/>
-      <c r="J75" s="101"/>
+      <c r="B75" s="102"/>
+      <c r="C75" s="103"/>
+      <c r="D75" s="103"/>
+      <c r="E75" s="103"/>
+      <c r="F75" s="103"/>
+      <c r="G75" s="103"/>
+      <c r="H75" s="103"/>
+      <c r="I75" s="103"/>
+      <c r="J75" s="104"/>
       <c r="K75" s="65"/>
       <c r="U75" s="10"/>
       <c r="V75" s="10"/>
     </row>
     <row r="76" spans="1:22" ht="13.2" customHeight="1">
       <c r="A76" s="109"/>
-      <c r="B76" s="88">
+      <c r="B76" s="81">
         <v>3</v>
       </c>
-      <c r="C76" s="76">
+      <c r="C76" s="90">
         <v>43468</v>
       </c>
-      <c r="D76" s="82">
+      <c r="D76" s="84">
         <v>43677</v>
       </c>
       <c r="E76" s="48">
@@ -8431,71 +8431,71 @@
       </c>
       <c r="F76" s="50"/>
       <c r="G76" s="53"/>
-      <c r="H76" s="82"/>
-      <c r="I76" s="88">
+      <c r="H76" s="84"/>
+      <c r="I76" s="81">
         <v>4</v>
       </c>
-      <c r="J76" s="88"/>
+      <c r="J76" s="81"/>
       <c r="K76" s="65"/>
       <c r="U76" s="10"/>
       <c r="V76" s="10"/>
     </row>
     <row r="77" spans="1:22" ht="13.2" customHeight="1">
       <c r="A77" s="109"/>
-      <c r="B77" s="89"/>
-      <c r="C77" s="77"/>
-      <c r="D77" s="83"/>
+      <c r="B77" s="82"/>
+      <c r="C77" s="91"/>
+      <c r="D77" s="85"/>
       <c r="E77" s="48">
         <v>43678</v>
       </c>
       <c r="F77" s="50"/>
       <c r="G77" s="53"/>
-      <c r="H77" s="83"/>
-      <c r="I77" s="89"/>
-      <c r="J77" s="89"/>
+      <c r="H77" s="85"/>
+      <c r="I77" s="82"/>
+      <c r="J77" s="82"/>
       <c r="K77" s="65"/>
       <c r="U77" s="10"/>
       <c r="V77" s="10"/>
     </row>
     <row r="78" spans="1:22" ht="13.2" customHeight="1">
       <c r="A78" s="109"/>
-      <c r="B78" s="89"/>
-      <c r="C78" s="77"/>
-      <c r="D78" s="83"/>
+      <c r="B78" s="82"/>
+      <c r="C78" s="91"/>
+      <c r="D78" s="85"/>
       <c r="E78" s="48">
-        <v>43705</v>
+        <v>43707</v>
       </c>
       <c r="F78" s="50"/>
       <c r="G78" s="53"/>
-      <c r="H78" s="83"/>
-      <c r="I78" s="89"/>
-      <c r="J78" s="89"/>
+      <c r="H78" s="85"/>
+      <c r="I78" s="82"/>
+      <c r="J78" s="82"/>
       <c r="K78" s="65"/>
       <c r="U78" s="10"/>
       <c r="V78" s="10"/>
     </row>
     <row r="79" spans="1:22" ht="13.2" customHeight="1">
       <c r="A79" s="109"/>
-      <c r="B79" s="89"/>
-      <c r="C79" s="78"/>
-      <c r="D79" s="84"/>
+      <c r="B79" s="82"/>
+      <c r="C79" s="92"/>
+      <c r="D79" s="86"/>
       <c r="E79" s="53"/>
       <c r="F79" s="53"/>
       <c r="G79" s="53"/>
-      <c r="H79" s="84"/>
-      <c r="I79" s="90"/>
-      <c r="J79" s="90"/>
+      <c r="H79" s="86"/>
+      <c r="I79" s="83"/>
+      <c r="J79" s="83"/>
       <c r="K79" s="65"/>
       <c r="U79" s="10"/>
       <c r="V79" s="10"/>
     </row>
     <row r="80" spans="1:22" ht="13.2" customHeight="1">
       <c r="A80" s="109"/>
-      <c r="B80" s="89"/>
-      <c r="C80" s="76">
+      <c r="B80" s="82"/>
+      <c r="C80" s="90">
         <v>43499</v>
       </c>
-      <c r="D80" s="82">
+      <c r="D80" s="84">
         <v>43680</v>
       </c>
       <c r="E80" s="48">
@@ -8503,13 +8503,13 @@
       </c>
       <c r="F80" s="53"/>
       <c r="G80" s="45"/>
-      <c r="H80" s="82">
+      <c r="H80" s="84">
         <v>43678</v>
       </c>
-      <c r="I80" s="88">
+      <c r="I80" s="81">
         <v>3</v>
       </c>
-      <c r="J80" s="88">
+      <c r="J80" s="81">
         <v>1</v>
       </c>
       <c r="K80" s="65"/>
@@ -8518,45 +8518,45 @@
     </row>
     <row r="81" spans="1:22" ht="13.2" customHeight="1">
       <c r="A81" s="109"/>
-      <c r="B81" s="89"/>
-      <c r="C81" s="77"/>
-      <c r="D81" s="83"/>
+      <c r="B81" s="82"/>
+      <c r="C81" s="91"/>
+      <c r="D81" s="85"/>
       <c r="E81" s="53"/>
       <c r="F81" s="53"/>
       <c r="G81" s="53"/>
-      <c r="H81" s="83"/>
-      <c r="I81" s="89"/>
-      <c r="J81" s="89"/>
+      <c r="H81" s="85"/>
+      <c r="I81" s="82"/>
+      <c r="J81" s="82"/>
       <c r="K81" s="65"/>
       <c r="U81" s="10"/>
       <c r="V81" s="10"/>
     </row>
     <row r="82" spans="1:22" ht="13.2" customHeight="1">
       <c r="A82" s="109"/>
-      <c r="B82" s="89"/>
-      <c r="C82" s="77"/>
-      <c r="D82" s="83"/>
+      <c r="B82" s="82"/>
+      <c r="C82" s="91"/>
+      <c r="D82" s="85"/>
       <c r="E82" s="53"/>
       <c r="F82" s="53"/>
       <c r="G82" s="53"/>
-      <c r="H82" s="83"/>
-      <c r="I82" s="89"/>
-      <c r="J82" s="89"/>
+      <c r="H82" s="85"/>
+      <c r="I82" s="82"/>
+      <c r="J82" s="82"/>
       <c r="K82" s="65"/>
       <c r="U82" s="10"/>
       <c r="V82" s="10"/>
     </row>
     <row r="83" spans="1:22" ht="13.2" customHeight="1">
       <c r="A83" s="110"/>
-      <c r="B83" s="90"/>
-      <c r="C83" s="78"/>
-      <c r="D83" s="84"/>
+      <c r="B83" s="83"/>
+      <c r="C83" s="92"/>
+      <c r="D83" s="86"/>
       <c r="E83" s="53"/>
       <c r="F83" s="53"/>
       <c r="G83" s="53"/>
-      <c r="H83" s="84"/>
-      <c r="I83" s="90"/>
-      <c r="J83" s="90"/>
+      <c r="H83" s="86"/>
+      <c r="I83" s="83"/>
+      <c r="J83" s="83"/>
       <c r="K83" s="65"/>
       <c r="U83" s="10"/>
       <c r="V83" s="10"/>
@@ -8580,13 +8580,13 @@
       <c r="A85" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="B85" s="88">
+      <c r="B85" s="81">
         <v>1</v>
       </c>
-      <c r="C85" s="88" t="s">
+      <c r="C85" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="D85" s="82">
+      <c r="D85" s="84">
         <v>43687</v>
       </c>
       <c r="E85" s="48">
@@ -8594,13 +8594,13 @@
       </c>
       <c r="F85" s="63"/>
       <c r="G85" s="60"/>
-      <c r="H85" s="82">
+      <c r="H85" s="84">
         <v>43681</v>
       </c>
-      <c r="I85" s="88">
+      <c r="I85" s="81">
         <v>7</v>
       </c>
-      <c r="J85" s="88">
+      <c r="J85" s="81">
         <v>1</v>
       </c>
       <c r="K85" s="65"/>
@@ -8609,127 +8609,127 @@
     </row>
     <row r="86" spans="1:22" ht="13.2" customHeight="1">
       <c r="A86" s="109"/>
-      <c r="B86" s="89"/>
-      <c r="C86" s="89"/>
-      <c r="D86" s="83"/>
+      <c r="B86" s="82"/>
+      <c r="C86" s="82"/>
+      <c r="D86" s="85"/>
       <c r="E86" s="48"/>
       <c r="F86" s="63"/>
       <c r="G86" s="39"/>
-      <c r="H86" s="83"/>
-      <c r="I86" s="89"/>
-      <c r="J86" s="89"/>
+      <c r="H86" s="85"/>
+      <c r="I86" s="82"/>
+      <c r="J86" s="82"/>
       <c r="K86" s="65"/>
       <c r="U86" s="10"/>
       <c r="V86" s="10"/>
     </row>
     <row r="87" spans="1:22" ht="13.2" customHeight="1">
       <c r="A87" s="109"/>
-      <c r="B87" s="89"/>
-      <c r="C87" s="89"/>
-      <c r="D87" s="83"/>
+      <c r="B87" s="82"/>
+      <c r="C87" s="82"/>
+      <c r="D87" s="85"/>
       <c r="E87" s="39"/>
       <c r="F87" s="39"/>
       <c r="G87" s="39"/>
-      <c r="H87" s="83"/>
-      <c r="I87" s="89"/>
-      <c r="J87" s="89"/>
+      <c r="H87" s="85"/>
+      <c r="I87" s="82"/>
+      <c r="J87" s="82"/>
       <c r="K87" s="65"/>
       <c r="U87" s="10"/>
       <c r="V87" s="10"/>
     </row>
     <row r="88" spans="1:22" ht="13.2" customHeight="1">
       <c r="A88" s="109"/>
-      <c r="B88" s="89"/>
-      <c r="C88" s="89"/>
-      <c r="D88" s="83"/>
+      <c r="B88" s="82"/>
+      <c r="C88" s="82"/>
+      <c r="D88" s="85"/>
       <c r="E88" s="39"/>
       <c r="F88" s="39"/>
       <c r="G88" s="39"/>
-      <c r="H88" s="83"/>
-      <c r="I88" s="89"/>
-      <c r="J88" s="89"/>
+      <c r="H88" s="85"/>
+      <c r="I88" s="82"/>
+      <c r="J88" s="82"/>
       <c r="K88" s="65"/>
       <c r="V88" s="10"/>
     </row>
     <row r="89" spans="1:22" ht="13.2" customHeight="1">
       <c r="A89" s="109"/>
-      <c r="B89" s="89"/>
-      <c r="C89" s="89"/>
-      <c r="D89" s="83"/>
+      <c r="B89" s="82"/>
+      <c r="C89" s="82"/>
+      <c r="D89" s="85"/>
       <c r="E89" s="39"/>
       <c r="F89" s="39"/>
       <c r="G89" s="39"/>
-      <c r="H89" s="83"/>
-      <c r="I89" s="89"/>
-      <c r="J89" s="89"/>
+      <c r="H89" s="85"/>
+      <c r="I89" s="82"/>
+      <c r="J89" s="82"/>
       <c r="K89" s="65"/>
       <c r="V89" s="10"/>
     </row>
     <row r="90" spans="1:22" ht="13.2" customHeight="1">
       <c r="A90" s="109"/>
-      <c r="B90" s="89"/>
-      <c r="C90" s="89"/>
-      <c r="D90" s="83"/>
+      <c r="B90" s="82"/>
+      <c r="C90" s="82"/>
+      <c r="D90" s="85"/>
       <c r="E90" s="39"/>
       <c r="F90" s="39"/>
       <c r="G90" s="39"/>
-      <c r="H90" s="83"/>
-      <c r="I90" s="89"/>
-      <c r="J90" s="89"/>
+      <c r="H90" s="85"/>
+      <c r="I90" s="82"/>
+      <c r="J90" s="82"/>
       <c r="K90" s="65"/>
       <c r="V90" s="10"/>
     </row>
     <row r="91" spans="1:22" ht="13.2" customHeight="1">
       <c r="A91" s="109"/>
-      <c r="B91" s="89"/>
-      <c r="C91" s="89"/>
-      <c r="D91" s="83"/>
+      <c r="B91" s="82"/>
+      <c r="C91" s="82"/>
+      <c r="D91" s="85"/>
       <c r="E91" s="39"/>
       <c r="F91" s="39"/>
       <c r="G91" s="39"/>
-      <c r="H91" s="83"/>
-      <c r="I91" s="89"/>
-      <c r="J91" s="89"/>
+      <c r="H91" s="85"/>
+      <c r="I91" s="82"/>
+      <c r="J91" s="82"/>
       <c r="K91" s="65"/>
       <c r="V91" s="10"/>
     </row>
     <row r="92" spans="1:22" ht="13.2" customHeight="1">
       <c r="A92" s="109"/>
-      <c r="B92" s="90"/>
-      <c r="C92" s="90"/>
-      <c r="D92" s="84"/>
+      <c r="B92" s="83"/>
+      <c r="C92" s="83"/>
+      <c r="D92" s="86"/>
       <c r="E92" s="39"/>
       <c r="F92" s="39"/>
       <c r="G92" s="39"/>
-      <c r="H92" s="84"/>
-      <c r="I92" s="90"/>
-      <c r="J92" s="90"/>
+      <c r="H92" s="86"/>
+      <c r="I92" s="83"/>
+      <c r="J92" s="83"/>
       <c r="K92" s="65"/>
       <c r="V92" s="10"/>
     </row>
     <row r="93" spans="1:22" ht="13.2" customHeight="1">
       <c r="A93" s="109"/>
-      <c r="B93" s="85"/>
-      <c r="C93" s="86"/>
-      <c r="D93" s="86"/>
-      <c r="E93" s="86"/>
-      <c r="F93" s="86"/>
-      <c r="G93" s="86"/>
-      <c r="H93" s="86"/>
-      <c r="I93" s="86"/>
-      <c r="J93" s="87"/>
+      <c r="B93" s="78"/>
+      <c r="C93" s="79"/>
+      <c r="D93" s="79"/>
+      <c r="E93" s="79"/>
+      <c r="F93" s="79"/>
+      <c r="G93" s="79"/>
+      <c r="H93" s="79"/>
+      <c r="I93" s="79"/>
+      <c r="J93" s="80"/>
       <c r="K93" s="65"/>
       <c r="V93" s="10"/>
     </row>
     <row r="94" spans="1:22" ht="13.2" customHeight="1">
       <c r="A94" s="109"/>
-      <c r="B94" s="88">
+      <c r="B94" s="81">
         <v>2</v>
       </c>
-      <c r="C94" s="76">
+      <c r="C94" s="90">
         <v>43467</v>
       </c>
-      <c r="D94" s="79">
+      <c r="D94" s="87">
         <v>43690</v>
       </c>
       <c r="E94" s="54">
@@ -8737,13 +8737,13 @@
       </c>
       <c r="F94" s="44"/>
       <c r="G94" s="60"/>
-      <c r="H94" s="82">
+      <c r="H94" s="84">
         <v>43688</v>
       </c>
-      <c r="I94" s="88">
+      <c r="I94" s="81">
         <v>3</v>
       </c>
-      <c r="J94" s="88">
+      <c r="J94" s="81">
         <v>1</v>
       </c>
       <c r="K94" s="65"/>
@@ -8751,51 +8751,51 @@
     </row>
     <row r="95" spans="1:22" ht="13.2" customHeight="1">
       <c r="A95" s="109"/>
-      <c r="B95" s="89"/>
-      <c r="C95" s="77"/>
-      <c r="D95" s="80"/>
+      <c r="B95" s="82"/>
+      <c r="C95" s="91"/>
+      <c r="D95" s="88"/>
       <c r="E95" s="54"/>
       <c r="F95" s="44"/>
       <c r="G95" s="39"/>
-      <c r="H95" s="83"/>
-      <c r="I95" s="89"/>
-      <c r="J95" s="89"/>
+      <c r="H95" s="85"/>
+      <c r="I95" s="82"/>
+      <c r="J95" s="82"/>
       <c r="K95" s="65"/>
       <c r="V95" s="10"/>
     </row>
     <row r="96" spans="1:22" ht="13.2" customHeight="1">
       <c r="A96" s="109"/>
-      <c r="B96" s="89"/>
-      <c r="C96" s="77"/>
-      <c r="D96" s="80"/>
+      <c r="B96" s="82"/>
+      <c r="C96" s="91"/>
+      <c r="D96" s="88"/>
       <c r="E96" s="54"/>
       <c r="F96" s="44"/>
-      <c r="H96" s="83"/>
-      <c r="I96" s="89"/>
-      <c r="J96" s="89"/>
+      <c r="H96" s="85"/>
+      <c r="I96" s="82"/>
+      <c r="J96" s="82"/>
       <c r="K96" s="65"/>
       <c r="V96" s="10"/>
     </row>
     <row r="97" spans="1:11" ht="13.2" customHeight="1">
       <c r="A97" s="109"/>
-      <c r="B97" s="89"/>
-      <c r="C97" s="78"/>
-      <c r="D97" s="81"/>
+      <c r="B97" s="82"/>
+      <c r="C97" s="92"/>
+      <c r="D97" s="89"/>
       <c r="E97" s="39"/>
       <c r="F97" s="39"/>
       <c r="G97" s="39"/>
-      <c r="H97" s="84"/>
-      <c r="I97" s="90"/>
-      <c r="J97" s="90"/>
+      <c r="H97" s="86"/>
+      <c r="I97" s="83"/>
+      <c r="J97" s="83"/>
       <c r="K97" s="65"/>
     </row>
     <row r="98" spans="1:11" ht="13.2" customHeight="1">
       <c r="A98" s="109"/>
-      <c r="B98" s="89"/>
-      <c r="C98" s="76">
+      <c r="B98" s="82"/>
+      <c r="C98" s="90">
         <v>43498</v>
       </c>
-      <c r="D98" s="79">
+      <c r="D98" s="87">
         <v>43693</v>
       </c>
       <c r="E98" s="54">
@@ -8803,78 +8803,78 @@
       </c>
       <c r="F98" s="62"/>
       <c r="G98" s="60"/>
-      <c r="H98" s="82">
+      <c r="H98" s="84">
         <v>43691</v>
       </c>
-      <c r="I98" s="88">
+      <c r="I98" s="81">
         <v>3</v>
       </c>
-      <c r="J98" s="88">
+      <c r="J98" s="81">
         <v>1</v>
       </c>
       <c r="K98" s="65"/>
     </row>
     <row r="99" spans="1:11" ht="13.2" customHeight="1">
       <c r="A99" s="109"/>
-      <c r="B99" s="89"/>
-      <c r="C99" s="77"/>
-      <c r="D99" s="80"/>
+      <c r="B99" s="82"/>
+      <c r="C99" s="91"/>
+      <c r="D99" s="88"/>
       <c r="E99" s="54"/>
       <c r="F99" s="62"/>
       <c r="G99" s="39"/>
-      <c r="H99" s="83"/>
-      <c r="I99" s="89"/>
-      <c r="J99" s="89"/>
+      <c r="H99" s="85"/>
+      <c r="I99" s="82"/>
+      <c r="J99" s="82"/>
       <c r="K99" s="65"/>
     </row>
     <row r="100" spans="1:11" ht="13.2" customHeight="1">
       <c r="A100" s="109"/>
-      <c r="B100" s="89"/>
-      <c r="C100" s="77"/>
-      <c r="D100" s="80"/>
+      <c r="B100" s="82"/>
+      <c r="C100" s="91"/>
+      <c r="D100" s="88"/>
       <c r="E100" s="54"/>
       <c r="F100" s="62"/>
       <c r="G100" s="39"/>
-      <c r="H100" s="83"/>
-      <c r="I100" s="89"/>
-      <c r="J100" s="89"/>
+      <c r="H100" s="85"/>
+      <c r="I100" s="82"/>
+      <c r="J100" s="82"/>
       <c r="K100" s="65"/>
     </row>
     <row r="101" spans="1:11" ht="13.2" customHeight="1">
       <c r="A101" s="109"/>
-      <c r="B101" s="90"/>
-      <c r="C101" s="78"/>
-      <c r="D101" s="81"/>
+      <c r="B101" s="83"/>
+      <c r="C101" s="92"/>
+      <c r="D101" s="89"/>
       <c r="E101" s="39"/>
       <c r="F101" s="39"/>
       <c r="G101" s="39"/>
-      <c r="H101" s="84"/>
-      <c r="I101" s="90"/>
-      <c r="J101" s="90"/>
+      <c r="H101" s="86"/>
+      <c r="I101" s="83"/>
+      <c r="J101" s="83"/>
       <c r="K101" s="65"/>
     </row>
     <row r="102" spans="1:11" ht="13.2" customHeight="1">
       <c r="A102" s="109"/>
-      <c r="B102" s="85"/>
-      <c r="C102" s="86"/>
-      <c r="D102" s="86"/>
-      <c r="E102" s="86"/>
-      <c r="F102" s="86"/>
-      <c r="G102" s="86"/>
-      <c r="H102" s="86"/>
-      <c r="I102" s="86"/>
-      <c r="J102" s="87"/>
+      <c r="B102" s="78"/>
+      <c r="C102" s="79"/>
+      <c r="D102" s="79"/>
+      <c r="E102" s="79"/>
+      <c r="F102" s="79"/>
+      <c r="G102" s="79"/>
+      <c r="H102" s="79"/>
+      <c r="I102" s="79"/>
+      <c r="J102" s="80"/>
       <c r="K102" s="65"/>
     </row>
     <row r="103" spans="1:11" ht="13.2" customHeight="1">
       <c r="A103" s="109"/>
-      <c r="B103" s="88">
+      <c r="B103" s="81">
         <v>3</v>
       </c>
-      <c r="C103" s="76">
+      <c r="C103" s="90">
         <v>43468</v>
       </c>
-      <c r="D103" s="79">
+      <c r="D103" s="87">
         <v>43708</v>
       </c>
       <c r="E103" s="54">
@@ -8882,61 +8882,61 @@
       </c>
       <c r="F103" s="64"/>
       <c r="G103" s="39"/>
-      <c r="H103" s="82"/>
-      <c r="I103" s="105">
+      <c r="H103" s="84"/>
+      <c r="I103" s="96">
         <v>15</v>
       </c>
-      <c r="J103" s="88"/>
+      <c r="J103" s="81"/>
       <c r="K103" s="65"/>
     </row>
     <row r="104" spans="1:11" ht="13.2" customHeight="1">
       <c r="A104" s="109"/>
-      <c r="B104" s="89"/>
-      <c r="C104" s="77"/>
-      <c r="D104" s="80"/>
+      <c r="B104" s="82"/>
+      <c r="C104" s="91"/>
+      <c r="D104" s="88"/>
       <c r="E104" s="54">
-        <v>43705</v>
+        <v>43707</v>
       </c>
       <c r="F104" s="64"/>
       <c r="G104" s="39"/>
-      <c r="H104" s="83"/>
-      <c r="I104" s="106"/>
-      <c r="J104" s="89"/>
+      <c r="H104" s="85"/>
+      <c r="I104" s="97"/>
+      <c r="J104" s="82"/>
       <c r="K104" s="65"/>
     </row>
     <row r="105" spans="1:11" ht="13.2" customHeight="1">
       <c r="A105" s="109"/>
-      <c r="B105" s="89"/>
-      <c r="C105" s="77"/>
-      <c r="D105" s="80"/>
+      <c r="B105" s="82"/>
+      <c r="C105" s="91"/>
+      <c r="D105" s="88"/>
       <c r="E105" s="73"/>
       <c r="F105" s="39"/>
       <c r="G105" s="39"/>
-      <c r="H105" s="83"/>
-      <c r="I105" s="106"/>
-      <c r="J105" s="89"/>
+      <c r="H105" s="85"/>
+      <c r="I105" s="97"/>
+      <c r="J105" s="82"/>
       <c r="K105" s="65"/>
     </row>
     <row r="106" spans="1:11" ht="13.2" customHeight="1">
       <c r="A106" s="109"/>
-      <c r="B106" s="89"/>
-      <c r="C106" s="78"/>
-      <c r="D106" s="81"/>
+      <c r="B106" s="82"/>
+      <c r="C106" s="92"/>
+      <c r="D106" s="89"/>
       <c r="E106" s="39"/>
       <c r="F106" s="39"/>
       <c r="G106" s="39"/>
-      <c r="H106" s="84"/>
-      <c r="I106" s="107"/>
-      <c r="J106" s="90"/>
+      <c r="H106" s="86"/>
+      <c r="I106" s="98"/>
+      <c r="J106" s="83"/>
       <c r="K106" s="65"/>
     </row>
     <row r="107" spans="1:11" ht="13.2" customHeight="1">
       <c r="A107" s="109"/>
-      <c r="B107" s="89"/>
-      <c r="C107" s="76">
+      <c r="B107" s="82"/>
+      <c r="C107" s="90">
         <v>43499</v>
       </c>
-      <c r="D107" s="79">
+      <c r="D107" s="87">
         <v>43711</v>
       </c>
       <c r="E107" s="52">
@@ -8944,76 +8944,76 @@
       </c>
       <c r="F107" s="57"/>
       <c r="G107" s="62"/>
-      <c r="H107" s="82"/>
-      <c r="I107" s="88">
+      <c r="H107" s="84"/>
+      <c r="I107" s="81">
         <v>3</v>
       </c>
-      <c r="J107" s="88"/>
+      <c r="J107" s="81"/>
       <c r="K107" s="65"/>
     </row>
     <row r="108" spans="1:11" ht="13.2" customHeight="1">
       <c r="A108" s="109"/>
-      <c r="B108" s="89"/>
-      <c r="C108" s="77"/>
-      <c r="D108" s="80"/>
+      <c r="B108" s="82"/>
+      <c r="C108" s="91"/>
+      <c r="D108" s="88"/>
       <c r="E108" s="61"/>
       <c r="F108" s="39"/>
       <c r="G108" s="59"/>
-      <c r="H108" s="83"/>
-      <c r="I108" s="89"/>
-      <c r="J108" s="89"/>
+      <c r="H108" s="85"/>
+      <c r="I108" s="82"/>
+      <c r="J108" s="82"/>
       <c r="K108" s="65"/>
     </row>
     <row r="109" spans="1:11" ht="13.2" customHeight="1">
       <c r="A109" s="109"/>
-      <c r="B109" s="89"/>
-      <c r="C109" s="77"/>
-      <c r="D109" s="80"/>
+      <c r="B109" s="82"/>
+      <c r="C109" s="91"/>
+      <c r="D109" s="88"/>
       <c r="E109" s="61"/>
       <c r="F109" s="39"/>
       <c r="G109" s="39"/>
-      <c r="H109" s="83"/>
-      <c r="I109" s="89"/>
-      <c r="J109" s="89"/>
+      <c r="H109" s="85"/>
+      <c r="I109" s="82"/>
+      <c r="J109" s="82"/>
       <c r="K109" s="65"/>
     </row>
     <row r="110" spans="1:11" ht="13.2" customHeight="1">
       <c r="A110" s="110"/>
-      <c r="B110" s="90"/>
-      <c r="C110" s="78"/>
-      <c r="D110" s="81"/>
+      <c r="B110" s="83"/>
+      <c r="C110" s="92"/>
+      <c r="D110" s="89"/>
       <c r="E110" s="61"/>
       <c r="F110" s="39"/>
       <c r="G110" s="39"/>
-      <c r="H110" s="84"/>
-      <c r="I110" s="90"/>
-      <c r="J110" s="90"/>
+      <c r="H110" s="86"/>
+      <c r="I110" s="83"/>
+      <c r="J110" s="83"/>
       <c r="K110" s="65"/>
     </row>
     <row r="111" spans="1:11" ht="13.2" customHeight="1">
-      <c r="A111" s="96"/>
-      <c r="B111" s="97"/>
-      <c r="C111" s="97"/>
-      <c r="D111" s="97"/>
-      <c r="E111" s="97"/>
-      <c r="F111" s="97"/>
-      <c r="G111" s="97"/>
-      <c r="H111" s="97"/>
-      <c r="I111" s="97"/>
-      <c r="J111" s="98"/>
+      <c r="A111" s="99"/>
+      <c r="B111" s="100"/>
+      <c r="C111" s="100"/>
+      <c r="D111" s="100"/>
+      <c r="E111" s="100"/>
+      <c r="F111" s="100"/>
+      <c r="G111" s="100"/>
+      <c r="H111" s="100"/>
+      <c r="I111" s="100"/>
+      <c r="J111" s="101"/>
       <c r="K111" s="65"/>
     </row>
     <row r="112" spans="1:11" ht="13.2" customHeight="1">
       <c r="A112" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="B112" s="88">
+      <c r="B112" s="81">
         <v>1</v>
       </c>
-      <c r="C112" s="88" t="s">
+      <c r="C112" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="D112" s="79">
+      <c r="D112" s="87">
         <v>43718</v>
       </c>
       <c r="E112" s="47">
@@ -9021,126 +9021,126 @@
       </c>
       <c r="F112" s="39"/>
       <c r="G112" s="39"/>
-      <c r="H112" s="82"/>
-      <c r="I112" s="88">
+      <c r="H112" s="84"/>
+      <c r="I112" s="81">
         <v>7</v>
       </c>
-      <c r="J112" s="88"/>
+      <c r="J112" s="81"/>
       <c r="K112" s="65"/>
     </row>
     <row r="113" spans="1:11" ht="13.2" customHeight="1">
       <c r="A113" s="109"/>
-      <c r="B113" s="89"/>
-      <c r="C113" s="89"/>
-      <c r="D113" s="80"/>
+      <c r="B113" s="82"/>
+      <c r="C113" s="82"/>
+      <c r="D113" s="88"/>
       <c r="E113" s="39"/>
       <c r="F113" s="39"/>
       <c r="G113" s="39"/>
-      <c r="H113" s="83"/>
-      <c r="I113" s="89"/>
-      <c r="J113" s="89"/>
+      <c r="H113" s="85"/>
+      <c r="I113" s="82"/>
+      <c r="J113" s="82"/>
       <c r="K113" s="65"/>
     </row>
     <row r="114" spans="1:11" ht="13.2" customHeight="1">
       <c r="A114" s="109"/>
-      <c r="B114" s="89"/>
-      <c r="C114" s="89"/>
-      <c r="D114" s="80"/>
+      <c r="B114" s="82"/>
+      <c r="C114" s="82"/>
+      <c r="D114" s="88"/>
       <c r="E114" s="39"/>
       <c r="F114" s="39"/>
       <c r="G114" s="39"/>
-      <c r="H114" s="83"/>
-      <c r="I114" s="89"/>
-      <c r="J114" s="89"/>
+      <c r="H114" s="85"/>
+      <c r="I114" s="82"/>
+      <c r="J114" s="82"/>
       <c r="K114" s="65"/>
     </row>
     <row r="115" spans="1:11" ht="13.2" customHeight="1">
       <c r="A115" s="109"/>
-      <c r="B115" s="89"/>
-      <c r="C115" s="89"/>
-      <c r="D115" s="80"/>
+      <c r="B115" s="82"/>
+      <c r="C115" s="82"/>
+      <c r="D115" s="88"/>
       <c r="E115" s="39"/>
       <c r="F115" s="39"/>
       <c r="G115" s="39"/>
-      <c r="H115" s="83"/>
-      <c r="I115" s="89"/>
-      <c r="J115" s="89"/>
+      <c r="H115" s="85"/>
+      <c r="I115" s="82"/>
+      <c r="J115" s="82"/>
       <c r="K115" s="65"/>
     </row>
     <row r="116" spans="1:11" ht="13.2" customHeight="1">
       <c r="A116" s="109"/>
-      <c r="B116" s="89"/>
-      <c r="C116" s="89"/>
-      <c r="D116" s="80"/>
+      <c r="B116" s="82"/>
+      <c r="C116" s="82"/>
+      <c r="D116" s="88"/>
       <c r="E116" s="39"/>
       <c r="F116" s="39"/>
       <c r="G116" s="39"/>
-      <c r="H116" s="83"/>
-      <c r="I116" s="89"/>
-      <c r="J116" s="89"/>
+      <c r="H116" s="85"/>
+      <c r="I116" s="82"/>
+      <c r="J116" s="82"/>
       <c r="K116" s="65"/>
     </row>
     <row r="117" spans="1:11" ht="13.2" customHeight="1">
       <c r="A117" s="109"/>
-      <c r="B117" s="89"/>
-      <c r="C117" s="89"/>
-      <c r="D117" s="80"/>
+      <c r="B117" s="82"/>
+      <c r="C117" s="82"/>
+      <c r="D117" s="88"/>
       <c r="E117" s="39"/>
       <c r="F117" s="39"/>
       <c r="G117" s="39"/>
-      <c r="H117" s="83"/>
-      <c r="I117" s="89"/>
-      <c r="J117" s="89"/>
+      <c r="H117" s="85"/>
+      <c r="I117" s="82"/>
+      <c r="J117" s="82"/>
       <c r="K117" s="65"/>
     </row>
     <row r="118" spans="1:11" ht="13.2" customHeight="1">
       <c r="A118" s="109"/>
-      <c r="B118" s="89"/>
-      <c r="C118" s="89"/>
-      <c r="D118" s="80"/>
+      <c r="B118" s="82"/>
+      <c r="C118" s="82"/>
+      <c r="D118" s="88"/>
       <c r="E118" s="39"/>
       <c r="F118" s="39"/>
       <c r="G118" s="39"/>
-      <c r="H118" s="83"/>
-      <c r="I118" s="89"/>
-      <c r="J118" s="89"/>
+      <c r="H118" s="85"/>
+      <c r="I118" s="82"/>
+      <c r="J118" s="82"/>
       <c r="K118" s="65"/>
     </row>
     <row r="119" spans="1:11" ht="13.2" customHeight="1">
       <c r="A119" s="109"/>
-      <c r="B119" s="90"/>
-      <c r="C119" s="90"/>
-      <c r="D119" s="81"/>
+      <c r="B119" s="83"/>
+      <c r="C119" s="83"/>
+      <c r="D119" s="89"/>
       <c r="E119" s="39"/>
       <c r="F119" s="39"/>
       <c r="G119" s="39"/>
-      <c r="H119" s="84"/>
-      <c r="I119" s="90"/>
-      <c r="J119" s="90"/>
+      <c r="H119" s="86"/>
+      <c r="I119" s="83"/>
+      <c r="J119" s="83"/>
       <c r="K119" s="65"/>
     </row>
     <row r="120" spans="1:11" ht="13.2" customHeight="1">
       <c r="A120" s="109"/>
-      <c r="B120" s="85"/>
-      <c r="C120" s="86"/>
-      <c r="D120" s="86"/>
-      <c r="E120" s="86"/>
-      <c r="F120" s="86"/>
-      <c r="G120" s="86"/>
-      <c r="H120" s="86"/>
-      <c r="I120" s="86"/>
-      <c r="J120" s="87"/>
+      <c r="B120" s="78"/>
+      <c r="C120" s="79"/>
+      <c r="D120" s="79"/>
+      <c r="E120" s="79"/>
+      <c r="F120" s="79"/>
+      <c r="G120" s="79"/>
+      <c r="H120" s="79"/>
+      <c r="I120" s="79"/>
+      <c r="J120" s="80"/>
       <c r="K120" s="65"/>
     </row>
     <row r="121" spans="1:11" ht="13.2" customHeight="1">
       <c r="A121" s="109"/>
-      <c r="B121" s="88">
+      <c r="B121" s="81">
         <v>2</v>
       </c>
-      <c r="C121" s="76">
+      <c r="C121" s="90">
         <v>43467</v>
       </c>
-      <c r="D121" s="79">
+      <c r="D121" s="87">
         <v>43721</v>
       </c>
       <c r="E121" s="54">
@@ -9148,59 +9148,59 @@
       </c>
       <c r="F121" s="44"/>
       <c r="G121" s="39"/>
-      <c r="H121" s="82"/>
-      <c r="I121" s="88">
+      <c r="H121" s="84"/>
+      <c r="I121" s="81">
         <v>3</v>
       </c>
-      <c r="J121" s="88"/>
+      <c r="J121" s="81"/>
       <c r="K121" s="65"/>
     </row>
     <row r="122" spans="1:11" ht="13.2" customHeight="1">
       <c r="A122" s="109"/>
-      <c r="B122" s="89"/>
-      <c r="C122" s="77"/>
-      <c r="D122" s="80"/>
+      <c r="B122" s="82"/>
+      <c r="C122" s="91"/>
+      <c r="D122" s="88"/>
       <c r="E122" s="39"/>
       <c r="F122" s="39"/>
       <c r="G122" s="39"/>
-      <c r="H122" s="83"/>
-      <c r="I122" s="89"/>
-      <c r="J122" s="89"/>
+      <c r="H122" s="85"/>
+      <c r="I122" s="82"/>
+      <c r="J122" s="82"/>
       <c r="K122" s="65"/>
     </row>
     <row r="123" spans="1:11" ht="13.2" customHeight="1">
       <c r="A123" s="109"/>
-      <c r="B123" s="89"/>
-      <c r="C123" s="77"/>
-      <c r="D123" s="80"/>
+      <c r="B123" s="82"/>
+      <c r="C123" s="91"/>
+      <c r="D123" s="88"/>
       <c r="E123" s="39"/>
       <c r="F123" s="39"/>
       <c r="G123" s="39"/>
-      <c r="H123" s="83"/>
-      <c r="I123" s="89"/>
-      <c r="J123" s="89"/>
+      <c r="H123" s="85"/>
+      <c r="I123" s="82"/>
+      <c r="J123" s="82"/>
       <c r="K123" s="65"/>
     </row>
     <row r="124" spans="1:11" ht="13.2" customHeight="1">
       <c r="A124" s="109"/>
-      <c r="B124" s="89"/>
-      <c r="C124" s="78"/>
-      <c r="D124" s="81"/>
+      <c r="B124" s="82"/>
+      <c r="C124" s="92"/>
+      <c r="D124" s="89"/>
       <c r="E124" s="39"/>
       <c r="F124" s="39"/>
       <c r="G124" s="39"/>
-      <c r="H124" s="84"/>
-      <c r="I124" s="90"/>
-      <c r="J124" s="90"/>
+      <c r="H124" s="86"/>
+      <c r="I124" s="83"/>
+      <c r="J124" s="83"/>
       <c r="K124" s="65"/>
     </row>
     <row r="125" spans="1:11" ht="13.2" customHeight="1">
       <c r="A125" s="109"/>
-      <c r="B125" s="89"/>
-      <c r="C125" s="76">
+      <c r="B125" s="82"/>
+      <c r="C125" s="90">
         <v>43498</v>
       </c>
-      <c r="D125" s="79">
+      <c r="D125" s="87">
         <v>43724</v>
       </c>
       <c r="E125" s="47">
@@ -9208,74 +9208,74 @@
       </c>
       <c r="F125" s="39"/>
       <c r="G125" s="39"/>
-      <c r="H125" s="82"/>
-      <c r="I125" s="88">
+      <c r="H125" s="84"/>
+      <c r="I125" s="81">
         <v>3</v>
       </c>
-      <c r="J125" s="88"/>
+      <c r="J125" s="81"/>
       <c r="K125" s="65"/>
     </row>
     <row r="126" spans="1:11" ht="13.2" customHeight="1">
       <c r="A126" s="109"/>
-      <c r="B126" s="89"/>
-      <c r="C126" s="77"/>
-      <c r="D126" s="80"/>
+      <c r="B126" s="82"/>
+      <c r="C126" s="91"/>
+      <c r="D126" s="88"/>
       <c r="E126" s="39"/>
       <c r="F126" s="39"/>
       <c r="G126" s="39"/>
-      <c r="H126" s="83"/>
-      <c r="I126" s="89"/>
-      <c r="J126" s="89"/>
+      <c r="H126" s="85"/>
+      <c r="I126" s="82"/>
+      <c r="J126" s="82"/>
       <c r="K126" s="65"/>
     </row>
     <row r="127" spans="1:11" ht="13.2" customHeight="1">
       <c r="A127" s="109"/>
-      <c r="B127" s="89"/>
-      <c r="C127" s="77"/>
-      <c r="D127" s="80"/>
+      <c r="B127" s="82"/>
+      <c r="C127" s="91"/>
+      <c r="D127" s="88"/>
       <c r="E127" s="39"/>
       <c r="F127" s="39"/>
       <c r="G127" s="39"/>
-      <c r="H127" s="83"/>
-      <c r="I127" s="89"/>
-      <c r="J127" s="89"/>
+      <c r="H127" s="85"/>
+      <c r="I127" s="82"/>
+      <c r="J127" s="82"/>
       <c r="K127" s="65"/>
     </row>
     <row r="128" spans="1:11" ht="13.2" customHeight="1">
       <c r="A128" s="109"/>
-      <c r="B128" s="90"/>
-      <c r="C128" s="78"/>
-      <c r="D128" s="81"/>
+      <c r="B128" s="83"/>
+      <c r="C128" s="92"/>
+      <c r="D128" s="89"/>
       <c r="E128" s="39"/>
       <c r="F128" s="39"/>
       <c r="G128" s="39"/>
-      <c r="H128" s="84"/>
-      <c r="I128" s="90"/>
-      <c r="J128" s="90"/>
+      <c r="H128" s="86"/>
+      <c r="I128" s="83"/>
+      <c r="J128" s="83"/>
       <c r="K128" s="65"/>
     </row>
     <row r="129" spans="1:11" ht="13.2" customHeight="1">
       <c r="A129" s="109"/>
-      <c r="B129" s="85"/>
-      <c r="C129" s="86"/>
-      <c r="D129" s="86"/>
-      <c r="E129" s="86"/>
-      <c r="F129" s="86"/>
-      <c r="G129" s="86"/>
-      <c r="H129" s="86"/>
-      <c r="I129" s="86"/>
-      <c r="J129" s="87"/>
+      <c r="B129" s="78"/>
+      <c r="C129" s="79"/>
+      <c r="D129" s="79"/>
+      <c r="E129" s="79"/>
+      <c r="F129" s="79"/>
+      <c r="G129" s="79"/>
+      <c r="H129" s="79"/>
+      <c r="I129" s="79"/>
+      <c r="J129" s="80"/>
       <c r="K129" s="65"/>
     </row>
     <row r="130" spans="1:11" ht="13.2" customHeight="1">
       <c r="A130" s="109"/>
-      <c r="B130" s="88">
+      <c r="B130" s="81">
         <v>3</v>
       </c>
-      <c r="C130" s="76">
+      <c r="C130" s="90">
         <v>43468</v>
       </c>
-      <c r="D130" s="79">
+      <c r="D130" s="87">
         <v>43739</v>
       </c>
       <c r="E130" s="47">
@@ -9283,59 +9283,59 @@
       </c>
       <c r="F130" s="39"/>
       <c r="G130" s="39"/>
-      <c r="H130" s="82"/>
-      <c r="I130" s="105">
+      <c r="H130" s="84"/>
+      <c r="I130" s="96">
         <v>15</v>
       </c>
-      <c r="J130" s="88"/>
+      <c r="J130" s="81"/>
       <c r="K130" s="65"/>
     </row>
     <row r="131" spans="1:11" ht="13.2" customHeight="1">
       <c r="A131" s="109"/>
-      <c r="B131" s="89"/>
-      <c r="C131" s="77"/>
-      <c r="D131" s="80"/>
+      <c r="B131" s="82"/>
+      <c r="C131" s="91"/>
+      <c r="D131" s="88"/>
       <c r="E131" s="39"/>
       <c r="F131" s="39"/>
       <c r="G131" s="39"/>
-      <c r="H131" s="83"/>
-      <c r="I131" s="106"/>
-      <c r="J131" s="89"/>
+      <c r="H131" s="85"/>
+      <c r="I131" s="97"/>
+      <c r="J131" s="82"/>
       <c r="K131" s="65"/>
     </row>
     <row r="132" spans="1:11" ht="13.2" customHeight="1">
       <c r="A132" s="109"/>
-      <c r="B132" s="89"/>
-      <c r="C132" s="77"/>
-      <c r="D132" s="80"/>
+      <c r="B132" s="82"/>
+      <c r="C132" s="91"/>
+      <c r="D132" s="88"/>
       <c r="E132" s="39"/>
       <c r="F132" s="39"/>
       <c r="G132" s="39"/>
-      <c r="H132" s="83"/>
-      <c r="I132" s="106"/>
-      <c r="J132" s="89"/>
+      <c r="H132" s="85"/>
+      <c r="I132" s="97"/>
+      <c r="J132" s="82"/>
       <c r="K132" s="65"/>
     </row>
     <row r="133" spans="1:11" ht="13.2" customHeight="1">
       <c r="A133" s="109"/>
-      <c r="B133" s="89"/>
-      <c r="C133" s="78"/>
-      <c r="D133" s="81"/>
+      <c r="B133" s="82"/>
+      <c r="C133" s="92"/>
+      <c r="D133" s="89"/>
       <c r="E133" s="39"/>
       <c r="F133" s="39"/>
       <c r="G133" s="39"/>
-      <c r="H133" s="84"/>
-      <c r="I133" s="107"/>
-      <c r="J133" s="90"/>
+      <c r="H133" s="86"/>
+      <c r="I133" s="98"/>
+      <c r="J133" s="83"/>
       <c r="K133" s="65"/>
     </row>
     <row r="134" spans="1:11" ht="13.2" customHeight="1">
       <c r="A134" s="109"/>
-      <c r="B134" s="89"/>
-      <c r="C134" s="76">
+      <c r="B134" s="82"/>
+      <c r="C134" s="90">
         <v>43499</v>
       </c>
-      <c r="D134" s="79">
+      <c r="D134" s="87">
         <v>43742</v>
       </c>
       <c r="E134" s="47">
@@ -9343,50 +9343,50 @@
       </c>
       <c r="F134" s="39"/>
       <c r="G134" s="39"/>
-      <c r="H134" s="82"/>
-      <c r="I134" s="88">
+      <c r="H134" s="84"/>
+      <c r="I134" s="81">
         <v>3</v>
       </c>
-      <c r="J134" s="88"/>
+      <c r="J134" s="81"/>
       <c r="K134" s="65"/>
     </row>
     <row r="135" spans="1:11" ht="13.2" customHeight="1">
       <c r="A135" s="109"/>
-      <c r="B135" s="89"/>
-      <c r="C135" s="77"/>
-      <c r="D135" s="80"/>
+      <c r="B135" s="82"/>
+      <c r="C135" s="91"/>
+      <c r="D135" s="88"/>
       <c r="E135" s="39"/>
       <c r="F135" s="39"/>
       <c r="G135" s="39"/>
-      <c r="H135" s="83"/>
-      <c r="I135" s="89"/>
-      <c r="J135" s="89"/>
+      <c r="H135" s="85"/>
+      <c r="I135" s="82"/>
+      <c r="J135" s="82"/>
       <c r="K135" s="65"/>
     </row>
     <row r="136" spans="1:11" ht="13.2" customHeight="1">
       <c r="A136" s="109"/>
-      <c r="B136" s="89"/>
-      <c r="C136" s="77"/>
-      <c r="D136" s="80"/>
+      <c r="B136" s="82"/>
+      <c r="C136" s="91"/>
+      <c r="D136" s="88"/>
       <c r="E136" s="39"/>
       <c r="F136" s="39"/>
       <c r="G136" s="39"/>
-      <c r="H136" s="83"/>
-      <c r="I136" s="89"/>
-      <c r="J136" s="89"/>
+      <c r="H136" s="85"/>
+      <c r="I136" s="82"/>
+      <c r="J136" s="82"/>
       <c r="K136" s="65"/>
     </row>
     <row r="137" spans="1:11" ht="13.2" customHeight="1">
       <c r="A137" s="110"/>
-      <c r="B137" s="90"/>
-      <c r="C137" s="78"/>
-      <c r="D137" s="81"/>
+      <c r="B137" s="83"/>
+      <c r="C137" s="92"/>
+      <c r="D137" s="89"/>
       <c r="E137" s="39"/>
       <c r="F137" s="39"/>
       <c r="G137" s="39"/>
-      <c r="H137" s="84"/>
-      <c r="I137" s="90"/>
-      <c r="J137" s="90"/>
+      <c r="H137" s="86"/>
+      <c r="I137" s="83"/>
+      <c r="J137" s="83"/>
       <c r="K137" s="65"/>
     </row>
     <row r="138" spans="1:11" ht="13.2" customHeight="1">
@@ -9406,13 +9406,13 @@
       <c r="A139" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="B139" s="88">
+      <c r="B139" s="81">
         <v>1</v>
       </c>
-      <c r="C139" s="88" t="s">
+      <c r="C139" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="D139" s="79">
+      <c r="D139" s="87">
         <v>43748</v>
       </c>
       <c r="E139" s="47">
@@ -9420,126 +9420,126 @@
       </c>
       <c r="F139" s="39"/>
       <c r="G139" s="39"/>
-      <c r="H139" s="82"/>
-      <c r="I139" s="88">
+      <c r="H139" s="84"/>
+      <c r="I139" s="81">
         <v>6</v>
       </c>
-      <c r="J139" s="88"/>
+      <c r="J139" s="81"/>
       <c r="K139" s="65"/>
     </row>
     <row r="140" spans="1:11" ht="13.2" customHeight="1">
       <c r="A140" s="134"/>
-      <c r="B140" s="89"/>
-      <c r="C140" s="89"/>
-      <c r="D140" s="80"/>
+      <c r="B140" s="82"/>
+      <c r="C140" s="82"/>
+      <c r="D140" s="88"/>
       <c r="E140" s="39"/>
       <c r="F140" s="39"/>
       <c r="G140" s="39"/>
-      <c r="H140" s="83"/>
-      <c r="I140" s="89"/>
-      <c r="J140" s="89"/>
+      <c r="H140" s="85"/>
+      <c r="I140" s="82"/>
+      <c r="J140" s="82"/>
       <c r="K140" s="65"/>
     </row>
     <row r="141" spans="1:11" ht="13.2" customHeight="1">
       <c r="A141" s="134"/>
-      <c r="B141" s="89"/>
-      <c r="C141" s="89"/>
-      <c r="D141" s="80"/>
+      <c r="B141" s="82"/>
+      <c r="C141" s="82"/>
+      <c r="D141" s="88"/>
       <c r="E141" s="39"/>
       <c r="F141" s="39"/>
       <c r="G141" s="39"/>
-      <c r="H141" s="83"/>
-      <c r="I141" s="89"/>
-      <c r="J141" s="89"/>
+      <c r="H141" s="85"/>
+      <c r="I141" s="82"/>
+      <c r="J141" s="82"/>
       <c r="K141" s="65"/>
     </row>
     <row r="142" spans="1:11" ht="13.2" customHeight="1">
       <c r="A142" s="134"/>
-      <c r="B142" s="89"/>
-      <c r="C142" s="89"/>
-      <c r="D142" s="80"/>
+      <c r="B142" s="82"/>
+      <c r="C142" s="82"/>
+      <c r="D142" s="88"/>
       <c r="E142" s="39"/>
       <c r="F142" s="39"/>
       <c r="G142" s="39"/>
-      <c r="H142" s="83"/>
-      <c r="I142" s="89"/>
-      <c r="J142" s="89"/>
+      <c r="H142" s="85"/>
+      <c r="I142" s="82"/>
+      <c r="J142" s="82"/>
       <c r="K142" s="65"/>
     </row>
     <row r="143" spans="1:11" ht="13.2" customHeight="1">
       <c r="A143" s="134"/>
-      <c r="B143" s="89"/>
-      <c r="C143" s="89"/>
-      <c r="D143" s="80"/>
+      <c r="B143" s="82"/>
+      <c r="C143" s="82"/>
+      <c r="D143" s="88"/>
       <c r="E143" s="39"/>
       <c r="F143" s="39"/>
       <c r="G143" s="39"/>
-      <c r="H143" s="83"/>
-      <c r="I143" s="89"/>
-      <c r="J143" s="89"/>
+      <c r="H143" s="85"/>
+      <c r="I143" s="82"/>
+      <c r="J143" s="82"/>
       <c r="K143" s="65"/>
     </row>
     <row r="144" spans="1:11" ht="13.2" customHeight="1">
       <c r="A144" s="134"/>
-      <c r="B144" s="89"/>
-      <c r="C144" s="89"/>
-      <c r="D144" s="80"/>
+      <c r="B144" s="82"/>
+      <c r="C144" s="82"/>
+      <c r="D144" s="88"/>
       <c r="E144" s="39"/>
       <c r="F144" s="39"/>
       <c r="G144" s="39"/>
-      <c r="H144" s="83"/>
-      <c r="I144" s="89"/>
-      <c r="J144" s="89"/>
+      <c r="H144" s="85"/>
+      <c r="I144" s="82"/>
+      <c r="J144" s="82"/>
       <c r="K144" s="65"/>
     </row>
     <row r="145" spans="1:11" ht="13.2" customHeight="1">
       <c r="A145" s="134"/>
-      <c r="B145" s="89"/>
-      <c r="C145" s="89"/>
-      <c r="D145" s="80"/>
+      <c r="B145" s="82"/>
+      <c r="C145" s="82"/>
+      <c r="D145" s="88"/>
       <c r="E145" s="39"/>
       <c r="F145" s="39"/>
       <c r="G145" s="39"/>
-      <c r="H145" s="83"/>
-      <c r="I145" s="89"/>
-      <c r="J145" s="89"/>
+      <c r="H145" s="85"/>
+      <c r="I145" s="82"/>
+      <c r="J145" s="82"/>
       <c r="K145" s="65"/>
     </row>
     <row r="146" spans="1:11" ht="13.2" customHeight="1">
       <c r="A146" s="134"/>
-      <c r="B146" s="90"/>
-      <c r="C146" s="90"/>
-      <c r="D146" s="81"/>
+      <c r="B146" s="83"/>
+      <c r="C146" s="83"/>
+      <c r="D146" s="89"/>
       <c r="E146" s="39"/>
       <c r="F146" s="39"/>
       <c r="G146" s="39"/>
-      <c r="H146" s="84"/>
-      <c r="I146" s="90"/>
-      <c r="J146" s="90"/>
+      <c r="H146" s="86"/>
+      <c r="I146" s="83"/>
+      <c r="J146" s="83"/>
       <c r="K146" s="65"/>
     </row>
     <row r="147" spans="1:11" ht="13.2" customHeight="1">
       <c r="A147" s="134"/>
-      <c r="B147" s="85"/>
-      <c r="C147" s="86"/>
-      <c r="D147" s="86"/>
-      <c r="E147" s="86"/>
-      <c r="F147" s="86"/>
-      <c r="G147" s="86"/>
-      <c r="H147" s="86"/>
-      <c r="I147" s="86"/>
-      <c r="J147" s="87"/>
+      <c r="B147" s="78"/>
+      <c r="C147" s="79"/>
+      <c r="D147" s="79"/>
+      <c r="E147" s="79"/>
+      <c r="F147" s="79"/>
+      <c r="G147" s="79"/>
+      <c r="H147" s="79"/>
+      <c r="I147" s="79"/>
+      <c r="J147" s="80"/>
       <c r="K147" s="65"/>
     </row>
     <row r="148" spans="1:11" ht="13.2" customHeight="1">
       <c r="A148" s="134"/>
-      <c r="B148" s="88">
+      <c r="B148" s="81">
         <v>2</v>
       </c>
-      <c r="C148" s="76">
+      <c r="C148" s="90">
         <v>43467</v>
       </c>
-      <c r="D148" s="79">
+      <c r="D148" s="87">
         <v>43751</v>
       </c>
       <c r="E148" s="54">
@@ -9547,59 +9547,59 @@
       </c>
       <c r="F148" s="44"/>
       <c r="G148" s="39"/>
-      <c r="H148" s="82"/>
-      <c r="I148" s="88">
+      <c r="H148" s="84"/>
+      <c r="I148" s="81">
         <v>3</v>
       </c>
-      <c r="J148" s="88"/>
+      <c r="J148" s="81"/>
       <c r="K148" s="65"/>
     </row>
     <row r="149" spans="1:11" ht="13.2" customHeight="1">
       <c r="A149" s="134"/>
-      <c r="B149" s="89"/>
-      <c r="C149" s="77"/>
-      <c r="D149" s="80"/>
+      <c r="B149" s="82"/>
+      <c r="C149" s="91"/>
+      <c r="D149" s="88"/>
       <c r="E149" s="39"/>
       <c r="F149" s="39"/>
       <c r="G149" s="39"/>
-      <c r="H149" s="83"/>
-      <c r="I149" s="89"/>
-      <c r="J149" s="89"/>
+      <c r="H149" s="85"/>
+      <c r="I149" s="82"/>
+      <c r="J149" s="82"/>
       <c r="K149" s="65"/>
     </row>
     <row r="150" spans="1:11" ht="13.2" customHeight="1">
       <c r="A150" s="134"/>
-      <c r="B150" s="89"/>
-      <c r="C150" s="77"/>
-      <c r="D150" s="80"/>
+      <c r="B150" s="82"/>
+      <c r="C150" s="91"/>
+      <c r="D150" s="88"/>
       <c r="E150" s="39"/>
       <c r="F150" s="39"/>
       <c r="G150" s="39"/>
-      <c r="H150" s="83"/>
-      <c r="I150" s="89"/>
-      <c r="J150" s="89"/>
+      <c r="H150" s="85"/>
+      <c r="I150" s="82"/>
+      <c r="J150" s="82"/>
       <c r="K150" s="65"/>
     </row>
     <row r="151" spans="1:11" ht="13.2" customHeight="1">
       <c r="A151" s="134"/>
-      <c r="B151" s="89"/>
-      <c r="C151" s="78"/>
-      <c r="D151" s="81"/>
+      <c r="B151" s="82"/>
+      <c r="C151" s="92"/>
+      <c r="D151" s="89"/>
       <c r="E151" s="39"/>
       <c r="F151" s="39"/>
       <c r="G151" s="39"/>
-      <c r="H151" s="84"/>
-      <c r="I151" s="89"/>
-      <c r="J151" s="90"/>
+      <c r="H151" s="86"/>
+      <c r="I151" s="82"/>
+      <c r="J151" s="83"/>
       <c r="K151" s="65"/>
     </row>
     <row r="152" spans="1:11" ht="13.2" customHeight="1">
       <c r="A152" s="134"/>
-      <c r="B152" s="89"/>
-      <c r="C152" s="76">
+      <c r="B152" s="82"/>
+      <c r="C152" s="90">
         <v>43498</v>
       </c>
-      <c r="D152" s="79">
+      <c r="D152" s="87">
         <v>43751</v>
       </c>
       <c r="E152" s="54">
@@ -9608,71 +9608,71 @@
       <c r="F152" s="39"/>
       <c r="G152" s="39"/>
       <c r="H152" s="136"/>
-      <c r="I152" s="89"/>
+      <c r="I152" s="82"/>
       <c r="J152" s="136"/>
       <c r="K152" s="65"/>
     </row>
     <row r="153" spans="1:11" ht="13.2" customHeight="1">
       <c r="A153" s="134"/>
-      <c r="B153" s="89"/>
-      <c r="C153" s="77"/>
-      <c r="D153" s="80"/>
+      <c r="B153" s="82"/>
+      <c r="C153" s="91"/>
+      <c r="D153" s="88"/>
       <c r="E153" s="39"/>
       <c r="F153" s="39"/>
       <c r="G153" s="39"/>
       <c r="H153" s="137"/>
-      <c r="I153" s="89"/>
+      <c r="I153" s="82"/>
       <c r="J153" s="137"/>
       <c r="K153" s="65"/>
     </row>
     <row r="154" spans="1:11" ht="13.2" customHeight="1">
       <c r="A154" s="134"/>
-      <c r="B154" s="89"/>
-      <c r="C154" s="77"/>
-      <c r="D154" s="80"/>
+      <c r="B154" s="82"/>
+      <c r="C154" s="91"/>
+      <c r="D154" s="88"/>
       <c r="E154" s="39"/>
       <c r="F154" s="39"/>
       <c r="G154" s="39"/>
       <c r="H154" s="137"/>
-      <c r="I154" s="89"/>
+      <c r="I154" s="82"/>
       <c r="J154" s="137"/>
       <c r="K154" s="65"/>
     </row>
     <row r="155" spans="1:11" ht="13.2" customHeight="1">
       <c r="A155" s="134"/>
-      <c r="B155" s="90"/>
-      <c r="C155" s="78"/>
-      <c r="D155" s="81"/>
+      <c r="B155" s="83"/>
+      <c r="C155" s="92"/>
+      <c r="D155" s="89"/>
       <c r="E155" s="39"/>
       <c r="F155" s="39"/>
       <c r="G155" s="39"/>
       <c r="H155" s="138"/>
-      <c r="I155" s="90"/>
+      <c r="I155" s="83"/>
       <c r="J155" s="138"/>
       <c r="K155" s="65"/>
     </row>
     <row r="156" spans="1:11" ht="13.2" customHeight="1">
       <c r="A156" s="134"/>
-      <c r="B156" s="85"/>
-      <c r="C156" s="86"/>
-      <c r="D156" s="86"/>
-      <c r="E156" s="86"/>
-      <c r="F156" s="86"/>
-      <c r="G156" s="86"/>
-      <c r="H156" s="86"/>
-      <c r="I156" s="86"/>
-      <c r="J156" s="87"/>
+      <c r="B156" s="78"/>
+      <c r="C156" s="79"/>
+      <c r="D156" s="79"/>
+      <c r="E156" s="79"/>
+      <c r="F156" s="79"/>
+      <c r="G156" s="79"/>
+      <c r="H156" s="79"/>
+      <c r="I156" s="79"/>
+      <c r="J156" s="80"/>
       <c r="K156" s="65"/>
     </row>
     <row r="157" spans="1:11" ht="13.2" customHeight="1">
       <c r="A157" s="134"/>
-      <c r="B157" s="88">
+      <c r="B157" s="81">
         <v>3</v>
       </c>
-      <c r="C157" s="76">
+      <c r="C157" s="90">
         <v>43468</v>
       </c>
-      <c r="D157" s="79">
+      <c r="D157" s="87">
         <v>43755</v>
       </c>
       <c r="E157" s="47">
@@ -9680,59 +9680,59 @@
       </c>
       <c r="F157" s="39"/>
       <c r="G157" s="39"/>
-      <c r="H157" s="82"/>
-      <c r="I157" s="105">
+      <c r="H157" s="84"/>
+      <c r="I157" s="96">
         <v>4</v>
       </c>
-      <c r="J157" s="88"/>
+      <c r="J157" s="81"/>
       <c r="K157" s="65"/>
     </row>
     <row r="158" spans="1:11" ht="13.2" customHeight="1">
       <c r="A158" s="134"/>
-      <c r="B158" s="89"/>
-      <c r="C158" s="77"/>
-      <c r="D158" s="80"/>
+      <c r="B158" s="82"/>
+      <c r="C158" s="91"/>
+      <c r="D158" s="88"/>
       <c r="E158" s="39"/>
       <c r="F158" s="39"/>
       <c r="G158" s="39"/>
-      <c r="H158" s="83"/>
-      <c r="I158" s="106"/>
-      <c r="J158" s="89"/>
+      <c r="H158" s="85"/>
+      <c r="I158" s="97"/>
+      <c r="J158" s="82"/>
       <c r="K158" s="65"/>
     </row>
     <row r="159" spans="1:11" ht="13.2" customHeight="1">
       <c r="A159" s="134"/>
-      <c r="B159" s="89"/>
-      <c r="C159" s="77"/>
-      <c r="D159" s="80"/>
+      <c r="B159" s="82"/>
+      <c r="C159" s="91"/>
+      <c r="D159" s="88"/>
       <c r="E159" s="39"/>
       <c r="F159" s="39"/>
       <c r="G159" s="39"/>
-      <c r="H159" s="83"/>
-      <c r="I159" s="106"/>
-      <c r="J159" s="89"/>
+      <c r="H159" s="85"/>
+      <c r="I159" s="97"/>
+      <c r="J159" s="82"/>
       <c r="K159" s="65"/>
     </row>
     <row r="160" spans="1:11" ht="13.2" customHeight="1">
       <c r="A160" s="134"/>
-      <c r="B160" s="89"/>
-      <c r="C160" s="78"/>
-      <c r="D160" s="81"/>
+      <c r="B160" s="82"/>
+      <c r="C160" s="92"/>
+      <c r="D160" s="89"/>
       <c r="E160" s="39"/>
       <c r="F160" s="39"/>
       <c r="G160" s="39"/>
-      <c r="H160" s="84"/>
-      <c r="I160" s="107"/>
-      <c r="J160" s="90"/>
+      <c r="H160" s="86"/>
+      <c r="I160" s="98"/>
+      <c r="J160" s="83"/>
       <c r="K160" s="65"/>
     </row>
     <row r="161" spans="1:11" ht="13.2" customHeight="1">
       <c r="A161" s="134"/>
-      <c r="B161" s="89"/>
-      <c r="C161" s="76">
+      <c r="B161" s="82"/>
+      <c r="C161" s="90">
         <v>43499</v>
       </c>
-      <c r="D161" s="79">
+      <c r="D161" s="87">
         <v>43758</v>
       </c>
       <c r="E161" s="47">
@@ -9740,50 +9740,50 @@
       </c>
       <c r="F161" s="39"/>
       <c r="G161" s="39"/>
-      <c r="H161" s="82"/>
-      <c r="I161" s="88">
+      <c r="H161" s="84"/>
+      <c r="I161" s="81">
         <v>3</v>
       </c>
-      <c r="J161" s="88"/>
+      <c r="J161" s="81"/>
       <c r="K161" s="65"/>
     </row>
     <row r="162" spans="1:11" ht="13.2" customHeight="1">
       <c r="A162" s="134"/>
-      <c r="B162" s="89"/>
-      <c r="C162" s="77"/>
-      <c r="D162" s="80"/>
+      <c r="B162" s="82"/>
+      <c r="C162" s="91"/>
+      <c r="D162" s="88"/>
       <c r="E162" s="39"/>
       <c r="F162" s="39"/>
       <c r="G162" s="39"/>
-      <c r="H162" s="83"/>
-      <c r="I162" s="89"/>
-      <c r="J162" s="89"/>
+      <c r="H162" s="85"/>
+      <c r="I162" s="82"/>
+      <c r="J162" s="82"/>
       <c r="K162" s="65"/>
     </row>
     <row r="163" spans="1:11" ht="13.2" customHeight="1">
       <c r="A163" s="134"/>
-      <c r="B163" s="89"/>
-      <c r="C163" s="77"/>
-      <c r="D163" s="80"/>
+      <c r="B163" s="82"/>
+      <c r="C163" s="91"/>
+      <c r="D163" s="88"/>
       <c r="E163" s="39"/>
       <c r="F163" s="39"/>
       <c r="G163" s="39"/>
-      <c r="H163" s="83"/>
-      <c r="I163" s="89"/>
-      <c r="J163" s="89"/>
+      <c r="H163" s="85"/>
+      <c r="I163" s="82"/>
+      <c r="J163" s="82"/>
       <c r="K163" s="65"/>
     </row>
     <row r="164" spans="1:11" ht="13.2" customHeight="1">
       <c r="A164" s="135"/>
-      <c r="B164" s="90"/>
-      <c r="C164" s="78"/>
-      <c r="D164" s="81"/>
+      <c r="B164" s="83"/>
+      <c r="C164" s="92"/>
+      <c r="D164" s="89"/>
       <c r="E164" s="39"/>
       <c r="F164" s="39"/>
       <c r="G164" s="39"/>
-      <c r="H164" s="84"/>
-      <c r="I164" s="90"/>
-      <c r="J164" s="90"/>
+      <c r="H164" s="86"/>
+      <c r="I164" s="83"/>
+      <c r="J164" s="83"/>
       <c r="K164" s="65"/>
     </row>
     <row r="165" spans="1:11" ht="13.2" customHeight="1">
@@ -9844,7 +9844,7 @@
       <c r="A169" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="B169" s="88">
+      <c r="B169" s="81">
         <v>3</v>
       </c>
       <c r="C169" s="129">
@@ -9865,7 +9865,7 @@
     </row>
     <row r="170" spans="1:11" ht="13.2" customHeight="1">
       <c r="A170" s="109"/>
-      <c r="B170" s="89"/>
+      <c r="B170" s="82"/>
       <c r="C170" s="130"/>
       <c r="D170" s="130"/>
       <c r="E170" s="51"/>
@@ -9878,7 +9878,7 @@
     </row>
     <row r="171" spans="1:11" ht="13.2" customHeight="1">
       <c r="A171" s="109"/>
-      <c r="B171" s="89"/>
+      <c r="B171" s="82"/>
       <c r="C171" s="130"/>
       <c r="D171" s="130"/>
       <c r="E171" s="51"/>
@@ -9891,7 +9891,7 @@
     </row>
     <row r="172" spans="1:11" ht="13.2" customHeight="1">
       <c r="A172" s="109"/>
-      <c r="B172" s="89"/>
+      <c r="B172" s="82"/>
       <c r="C172" s="130"/>
       <c r="D172" s="130"/>
       <c r="E172" s="51"/>
@@ -9904,60 +9904,60 @@
     </row>
     <row r="173" spans="1:11" ht="13.2" customHeight="1">
       <c r="A173" s="109"/>
-      <c r="B173" s="89"/>
-      <c r="C173" s="76">
+      <c r="B173" s="82"/>
+      <c r="C173" s="90">
         <v>43558</v>
       </c>
-      <c r="D173" s="79">
+      <c r="D173" s="87">
         <v>43764</v>
       </c>
       <c r="E173" s="51"/>
       <c r="F173" s="44"/>
       <c r="G173" s="53"/>
-      <c r="H173" s="82"/>
-      <c r="I173" s="88">
+      <c r="H173" s="84"/>
+      <c r="I173" s="81">
         <v>3</v>
       </c>
-      <c r="J173" s="88"/>
+      <c r="J173" s="81"/>
       <c r="K173" s="66"/>
     </row>
     <row r="174" spans="1:11" ht="13.2" customHeight="1">
       <c r="A174" s="109"/>
-      <c r="B174" s="89"/>
-      <c r="C174" s="77"/>
-      <c r="D174" s="80"/>
+      <c r="B174" s="82"/>
+      <c r="C174" s="91"/>
+      <c r="D174" s="88"/>
       <c r="E174" s="51"/>
       <c r="F174" s="44"/>
       <c r="G174" s="53"/>
-      <c r="H174" s="83"/>
-      <c r="I174" s="89"/>
-      <c r="J174" s="89"/>
+      <c r="H174" s="85"/>
+      <c r="I174" s="82"/>
+      <c r="J174" s="82"/>
       <c r="K174" s="66"/>
     </row>
     <row r="175" spans="1:11" s="57" customFormat="1" ht="13.2" customHeight="1">
       <c r="A175" s="109"/>
-      <c r="B175" s="89"/>
-      <c r="C175" s="77"/>
-      <c r="D175" s="80"/>
+      <c r="B175" s="82"/>
+      <c r="C175" s="91"/>
+      <c r="D175" s="88"/>
       <c r="E175" s="51"/>
       <c r="F175" s="44"/>
       <c r="G175" s="53"/>
-      <c r="H175" s="83"/>
-      <c r="I175" s="89"/>
-      <c r="J175" s="89"/>
+      <c r="H175" s="85"/>
+      <c r="I175" s="82"/>
+      <c r="J175" s="82"/>
       <c r="K175" s="66"/>
     </row>
     <row r="176" spans="1:11" ht="13.2" customHeight="1">
       <c r="A176" s="110"/>
-      <c r="B176" s="90"/>
-      <c r="C176" s="78"/>
-      <c r="D176" s="81"/>
+      <c r="B176" s="83"/>
+      <c r="C176" s="92"/>
+      <c r="D176" s="89"/>
       <c r="E176" s="51"/>
       <c r="F176" s="44"/>
       <c r="G176" s="53"/>
-      <c r="H176" s="84"/>
-      <c r="I176" s="90"/>
-      <c r="J176" s="90"/>
+      <c r="H176" s="86"/>
+      <c r="I176" s="83"/>
+      <c r="J176" s="83"/>
       <c r="K176" s="66"/>
     </row>
     <row r="177" spans="1:11" ht="13.2" customHeight="1">
@@ -9977,7 +9977,7 @@
       <c r="A178" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="B178" s="88">
+      <c r="B178" s="81">
         <v>3</v>
       </c>
       <c r="C178" s="129">
@@ -9998,7 +9998,7 @@
     </row>
     <row r="179" spans="1:11" ht="13.2" customHeight="1">
       <c r="A179" s="109"/>
-      <c r="B179" s="89"/>
+      <c r="B179" s="82"/>
       <c r="C179" s="130"/>
       <c r="D179" s="130"/>
       <c r="E179" s="51"/>
@@ -10011,7 +10011,7 @@
     </row>
     <row r="180" spans="1:11" ht="13.2" customHeight="1">
       <c r="A180" s="109"/>
-      <c r="B180" s="89"/>
+      <c r="B180" s="82"/>
       <c r="C180" s="130"/>
       <c r="D180" s="130"/>
       <c r="E180" s="51"/>
@@ -10024,7 +10024,7 @@
     </row>
     <row r="181" spans="1:11" ht="13.2" customHeight="1">
       <c r="A181" s="109"/>
-      <c r="B181" s="89"/>
+      <c r="B181" s="82"/>
       <c r="C181" s="130"/>
       <c r="D181" s="130"/>
       <c r="E181" s="51"/>
@@ -10037,60 +10037,60 @@
     </row>
     <row r="182" spans="1:11" ht="13.2" customHeight="1">
       <c r="A182" s="109"/>
-      <c r="B182" s="89"/>
-      <c r="C182" s="76">
+      <c r="B182" s="82"/>
+      <c r="C182" s="90">
         <v>43558</v>
       </c>
-      <c r="D182" s="82">
+      <c r="D182" s="84">
         <v>43770</v>
       </c>
       <c r="E182" s="51"/>
       <c r="F182" s="44"/>
       <c r="G182" s="53"/>
-      <c r="H182" s="82"/>
-      <c r="I182" s="88">
+      <c r="H182" s="84"/>
+      <c r="I182" s="81">
         <v>3</v>
       </c>
-      <c r="J182" s="88"/>
+      <c r="J182" s="81"/>
       <c r="K182" s="66"/>
     </row>
     <row r="183" spans="1:11" ht="13.2" customHeight="1">
       <c r="A183" s="109"/>
-      <c r="B183" s="89"/>
-      <c r="C183" s="77"/>
-      <c r="D183" s="83"/>
+      <c r="B183" s="82"/>
+      <c r="C183" s="91"/>
+      <c r="D183" s="85"/>
       <c r="E183" s="51"/>
       <c r="F183" s="44"/>
       <c r="G183" s="53"/>
-      <c r="H183" s="83"/>
-      <c r="I183" s="89"/>
-      <c r="J183" s="89"/>
+      <c r="H183" s="85"/>
+      <c r="I183" s="82"/>
+      <c r="J183" s="82"/>
       <c r="K183" s="66"/>
     </row>
     <row r="184" spans="1:11" s="57" customFormat="1" ht="13.2" customHeight="1">
       <c r="A184" s="109"/>
-      <c r="B184" s="89"/>
-      <c r="C184" s="77"/>
-      <c r="D184" s="83"/>
+      <c r="B184" s="82"/>
+      <c r="C184" s="91"/>
+      <c r="D184" s="85"/>
       <c r="E184" s="51"/>
       <c r="F184" s="44"/>
       <c r="G184" s="53"/>
-      <c r="H184" s="83"/>
-      <c r="I184" s="89"/>
-      <c r="J184" s="89"/>
+      <c r="H184" s="85"/>
+      <c r="I184" s="82"/>
+      <c r="J184" s="82"/>
       <c r="K184" s="66"/>
     </row>
     <row r="185" spans="1:11" ht="13.2" customHeight="1">
       <c r="A185" s="110"/>
-      <c r="B185" s="90"/>
-      <c r="C185" s="78"/>
-      <c r="D185" s="84"/>
+      <c r="B185" s="83"/>
+      <c r="C185" s="92"/>
+      <c r="D185" s="86"/>
       <c r="E185" s="51"/>
       <c r="F185" s="44"/>
       <c r="G185" s="53"/>
-      <c r="H185" s="84"/>
-      <c r="I185" s="90"/>
-      <c r="J185" s="90"/>
+      <c r="H185" s="86"/>
+      <c r="I185" s="83"/>
+      <c r="J185" s="83"/>
       <c r="K185" s="66"/>
     </row>
     <row r="186" spans="1:11" ht="13.2" customHeight="1">
@@ -10671,23 +10671,23 @@
       <c r="B225" s="151" t="s">
         <v>32</v>
       </c>
-      <c r="C225" s="92" t="s">
+      <c r="C225" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="D225" s="92" t="s">
+      <c r="D225" s="77" t="s">
         <v>7</v>
       </c>
       <c r="E225" s="125" t="s">
         <v>8</v>
       </c>
       <c r="F225" s="155"/>
-      <c r="G225" s="92" t="s">
+      <c r="G225" s="77" t="s">
         <v>9</v>
       </c>
       <c r="H225" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="I225" s="92" t="s">
+      <c r="I225" s="77" t="s">
         <v>12</v>
       </c>
       <c r="J225" s="66"/>
@@ -19694,8 +19694,6 @@
     <mergeCell ref="D218:D221"/>
     <mergeCell ref="H218:H221"/>
     <mergeCell ref="I218:I221"/>
-    <mergeCell ref="C49:C52"/>
-    <mergeCell ref="C53:C56"/>
     <mergeCell ref="B76:B83"/>
     <mergeCell ref="A58:A83"/>
     <mergeCell ref="B49:B56"/>
@@ -19707,6 +19705,8 @@
     <mergeCell ref="H40:H43"/>
     <mergeCell ref="D44:D47"/>
     <mergeCell ref="D40:D43"/>
+    <mergeCell ref="B40:B47"/>
+    <mergeCell ref="D31:D38"/>
     <mergeCell ref="J218:J221"/>
     <mergeCell ref="A196:A203"/>
     <mergeCell ref="A204:J204"/>
@@ -19731,9 +19731,6 @@
     <mergeCell ref="J196:J199"/>
     <mergeCell ref="C200:C203"/>
     <mergeCell ref="D200:D203"/>
-    <mergeCell ref="H200:H203"/>
-    <mergeCell ref="I200:I203"/>
-    <mergeCell ref="J200:J203"/>
     <mergeCell ref="A187:A194"/>
     <mergeCell ref="B187:B194"/>
     <mergeCell ref="C187:C190"/>
@@ -19746,7 +19743,18 @@
     <mergeCell ref="H191:H194"/>
     <mergeCell ref="I191:I194"/>
     <mergeCell ref="J191:J194"/>
+    <mergeCell ref="D173:D176"/>
+    <mergeCell ref="H173:H176"/>
+    <mergeCell ref="I173:I176"/>
+    <mergeCell ref="J173:J176"/>
+    <mergeCell ref="B139:B146"/>
+    <mergeCell ref="D139:D146"/>
+    <mergeCell ref="C139:C146"/>
+    <mergeCell ref="H200:H203"/>
+    <mergeCell ref="I200:I203"/>
+    <mergeCell ref="J200:J203"/>
     <mergeCell ref="A195:J195"/>
+    <mergeCell ref="J148:J151"/>
     <mergeCell ref="B147:J147"/>
     <mergeCell ref="B121:B128"/>
     <mergeCell ref="D112:D119"/>
@@ -19755,13 +19763,10 @@
     <mergeCell ref="H169:H172"/>
     <mergeCell ref="I169:I172"/>
     <mergeCell ref="J169:J172"/>
-    <mergeCell ref="D173:D176"/>
-    <mergeCell ref="H173:H176"/>
-    <mergeCell ref="I173:I176"/>
-    <mergeCell ref="J173:J176"/>
-    <mergeCell ref="B139:B146"/>
-    <mergeCell ref="D139:D146"/>
-    <mergeCell ref="C139:C146"/>
+    <mergeCell ref="H139:H146"/>
+    <mergeCell ref="B148:B155"/>
+    <mergeCell ref="H17:H20"/>
+    <mergeCell ref="B22:B29"/>
     <mergeCell ref="A169:A176"/>
     <mergeCell ref="B169:B176"/>
     <mergeCell ref="C173:C176"/>
@@ -19782,9 +19787,10 @@
     <mergeCell ref="D152:D155"/>
     <mergeCell ref="H148:H151"/>
     <mergeCell ref="H152:H155"/>
-    <mergeCell ref="J148:J151"/>
-    <mergeCell ref="B40:B47"/>
-    <mergeCell ref="D31:D38"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B31:B38"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="I4:I11"/>
     <mergeCell ref="A4:A29"/>
     <mergeCell ref="C178:C181"/>
     <mergeCell ref="D178:D181"/>
@@ -19805,12 +19811,15 @@
     <mergeCell ref="D148:D151"/>
     <mergeCell ref="I148:I155"/>
     <mergeCell ref="I139:I146"/>
-    <mergeCell ref="H139:H146"/>
-    <mergeCell ref="B148:B155"/>
-    <mergeCell ref="H17:H20"/>
-    <mergeCell ref="B22:B29"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J67:J70"/>
+    <mergeCell ref="J71:J74"/>
+    <mergeCell ref="J76:J79"/>
+    <mergeCell ref="J80:J83"/>
+    <mergeCell ref="I67:I74"/>
+    <mergeCell ref="D67:D70"/>
+    <mergeCell ref="D71:D74"/>
+    <mergeCell ref="H67:H70"/>
     <mergeCell ref="D80:D83"/>
     <mergeCell ref="D76:D79"/>
     <mergeCell ref="D26:D29"/>
@@ -19820,19 +19829,8 @@
     <mergeCell ref="D53:D56"/>
     <mergeCell ref="C80:C83"/>
     <mergeCell ref="C76:C79"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J67:J70"/>
-    <mergeCell ref="J71:J74"/>
-    <mergeCell ref="J76:J79"/>
-    <mergeCell ref="J80:J83"/>
-    <mergeCell ref="I67:I74"/>
-    <mergeCell ref="D67:D70"/>
-    <mergeCell ref="D71:D74"/>
-    <mergeCell ref="H67:H70"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B31:B38"/>
-    <mergeCell ref="H85:H92"/>
-    <mergeCell ref="C98:C101"/>
+    <mergeCell ref="C49:C52"/>
+    <mergeCell ref="C53:C56"/>
     <mergeCell ref="I107:I110"/>
     <mergeCell ref="M1:P6"/>
     <mergeCell ref="I22:I25"/>
@@ -19855,8 +19853,8 @@
     <mergeCell ref="D4:D11"/>
     <mergeCell ref="H22:H25"/>
     <mergeCell ref="D17:D20"/>
-    <mergeCell ref="D103:D106"/>
-    <mergeCell ref="B48:J48"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="A1:J1"/>
     <mergeCell ref="J13:J16"/>
     <mergeCell ref="A30:J30"/>
     <mergeCell ref="B39:J39"/>
@@ -19879,8 +19877,12 @@
     <mergeCell ref="B130:B137"/>
     <mergeCell ref="H98:H101"/>
     <mergeCell ref="H94:H97"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="I4:I11"/>
+    <mergeCell ref="H85:H92"/>
+    <mergeCell ref="C98:C101"/>
+    <mergeCell ref="D94:D97"/>
+    <mergeCell ref="D98:D101"/>
+    <mergeCell ref="J94:J97"/>
+    <mergeCell ref="I103:I106"/>
     <mergeCell ref="J26:J29"/>
     <mergeCell ref="J22:J25"/>
     <mergeCell ref="A57:J57"/>
@@ -19899,6 +19901,13 @@
     <mergeCell ref="H31:H38"/>
     <mergeCell ref="H26:H29"/>
     <mergeCell ref="I53:I56"/>
+    <mergeCell ref="D103:D106"/>
+    <mergeCell ref="B48:J48"/>
+    <mergeCell ref="D134:D137"/>
+    <mergeCell ref="H130:H133"/>
+    <mergeCell ref="B129:J129"/>
+    <mergeCell ref="C85:C92"/>
+    <mergeCell ref="D121:D124"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="C22:C25"/>
     <mergeCell ref="D49:D52"/>
@@ -19918,22 +19927,6 @@
     <mergeCell ref="I85:I92"/>
     <mergeCell ref="J98:J101"/>
     <mergeCell ref="B93:J93"/>
-    <mergeCell ref="D85:D92"/>
-    <mergeCell ref="D94:D97"/>
-    <mergeCell ref="D98:D101"/>
-    <mergeCell ref="J94:J97"/>
-    <mergeCell ref="I103:I106"/>
-    <mergeCell ref="J103:J106"/>
-    <mergeCell ref="J107:J110"/>
-    <mergeCell ref="C94:C97"/>
-    <mergeCell ref="B85:B92"/>
-    <mergeCell ref="C121:C124"/>
-    <mergeCell ref="C125:C128"/>
-    <mergeCell ref="D134:D137"/>
-    <mergeCell ref="H130:H133"/>
-    <mergeCell ref="B129:J129"/>
-    <mergeCell ref="C85:C92"/>
-    <mergeCell ref="D121:D124"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="B102:J102"/>
     <mergeCell ref="I98:I101"/>
@@ -19951,6 +19944,13 @@
     <mergeCell ref="H49:H52"/>
     <mergeCell ref="I49:I52"/>
     <mergeCell ref="J49:J52"/>
+    <mergeCell ref="J103:J106"/>
+    <mergeCell ref="J107:J110"/>
+    <mergeCell ref="C94:C97"/>
+    <mergeCell ref="B85:B92"/>
+    <mergeCell ref="C121:C124"/>
+    <mergeCell ref="C125:C128"/>
+    <mergeCell ref="D85:D92"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Registro de estado de progreso.xlsx
se actuliazo una entrega
</commit_message>
<xml_diff>
--- a/Documentos para el proyecto de Sanambiente/Registro de estado de progreso.xlsx
+++ b/Documentos para el proyecto de Sanambiente/Registro de estado de progreso.xlsx
@@ -8513,7 +8513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="305">
+  <cellXfs count="309">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -9323,6 +9323,10 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -31564,8 +31568,8 @@
   </sheetPr>
   <dimension ref="A1:P1089"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
-      <selection activeCell="C206" sqref="C206:C209"/>
+    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
+      <selection activeCell="G258" sqref="G258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -34892,8 +34896,10 @@
       <c r="D206" s="237">
         <v>43742</v>
       </c>
-      <c r="E206" s="81"/>
-      <c r="F206" s="81"/>
+      <c r="E206" s="96">
+        <v>43743</v>
+      </c>
+      <c r="F206" s="97"/>
       <c r="G206" s="81"/>
       <c r="H206" s="236"/>
       <c r="I206" s="236"/>
@@ -35536,8 +35542,10 @@
       <c r="D250" s="230">
         <v>43770</v>
       </c>
-      <c r="E250" s="69"/>
-      <c r="F250" s="69"/>
+      <c r="E250" s="305">
+        <v>43771</v>
+      </c>
+      <c r="F250" s="306"/>
       <c r="G250" s="69"/>
       <c r="H250" s="223"/>
       <c r="I250" s="223"/>
@@ -35593,8 +35601,10 @@
       <c r="D254" s="230">
         <v>43772</v>
       </c>
-      <c r="E254" s="69"/>
-      <c r="F254" s="69"/>
+      <c r="E254" s="305">
+        <v>43773</v>
+      </c>
+      <c r="F254" s="306"/>
       <c r="G254" s="69"/>
       <c r="H254" s="223"/>
       <c r="I254" s="223"/>
@@ -35649,9 +35659,11 @@
       <c r="D258" s="230">
         <v>43774</v>
       </c>
-      <c r="E258" s="69"/>
-      <c r="F258" s="69"/>
-      <c r="G258" s="69"/>
+      <c r="E258" s="305">
+        <v>43785</v>
+      </c>
+      <c r="F258" s="307"/>
+      <c r="G258" s="308"/>
       <c r="H258" s="223"/>
       <c r="I258" s="223"/>
       <c r="J258" s="223"/>
@@ -35720,8 +35732,10 @@
       <c r="D263" s="230">
         <v>43776</v>
       </c>
-      <c r="E263" s="69"/>
-      <c r="F263" s="69"/>
+      <c r="E263" s="305">
+        <v>43777</v>
+      </c>
+      <c r="F263" s="306"/>
       <c r="G263" s="69"/>
       <c r="H263" s="223"/>
       <c r="I263" s="223"/>

</xml_diff>